<commit_message>
Fixed header in questions-skill-models
</commit_message>
<xml_diff>
--- a/data/CAT_COMMANDS/questions-skill_model1b.xlsx
+++ b/data/CAT_COMMANDS/questions-skill_model1b.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgia/repositories/CAT-unplugged/model/data/CAT_COMMANDS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgia/repositories/virtual-CAT-itas/data/CAT_COMMANDS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFCE3C6-A914-DB46-AF03-307065BAE2F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAA3ED8-FC9A-4549-B8CE-01CC22F543FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33100" yWindow="-23020" windowWidth="38400" windowHeight="21100" xr2:uid="{3D5E00E8-EA45-C34D-85AA-17AD78DA61C2}"/>
+    <workbookView xWindow="27480" yWindow="-23020" windowWidth="38400" windowHeight="21100" xr2:uid="{3D5E00E8-EA45-C34D-85AA-17AD78DA61C2}"/>
   </bookViews>
   <sheets>
     <sheet name="question-skills-basic" sheetId="17" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="93">
   <si>
     <t>Question_ID</t>
   </si>
@@ -220,6 +220,99 @@
   </si>
   <si>
     <t>paintDot</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
+    <t>E9</t>
+  </si>
+  <si>
+    <t>E10</t>
+  </si>
+  <si>
+    <t>E11</t>
+  </si>
+  <si>
+    <t>E12</t>
+  </si>
+  <si>
+    <t>E13</t>
+  </si>
+  <si>
+    <t>E14</t>
+  </si>
+  <si>
+    <t>E15</t>
+  </si>
+  <si>
+    <t>E16</t>
+  </si>
+  <si>
+    <t>E17</t>
+  </si>
+  <si>
+    <t>E18</t>
+  </si>
+  <si>
+    <t>E19</t>
+  </si>
+  <si>
+    <t>E20</t>
+  </si>
+  <si>
+    <t>E21</t>
+  </si>
+  <si>
+    <t>E22</t>
+  </si>
+  <si>
+    <t>E23</t>
+  </si>
+  <si>
+    <t>E24</t>
+  </si>
+  <si>
+    <t>E25</t>
+  </si>
+  <si>
+    <t>E26</t>
+  </si>
+  <si>
+    <t>E27</t>
+  </si>
+  <si>
+    <t>E28</t>
+  </si>
+  <si>
+    <t>E29</t>
+  </si>
+  <si>
+    <t>E30</t>
+  </si>
+  <si>
+    <t>E31</t>
   </si>
 </sst>
 </file>
@@ -517,6 +610,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -524,9 +620,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -873,7 +966,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4:AH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1469,36 +1562,99 @@
       <c r="A4" s="50"/>
       <c r="B4" s="50"/>
       <c r="C4" s="50"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="5"/>
-      <c r="Z4" s="5"/>
-      <c r="AA4" s="5"/>
-      <c r="AB4" s="5"/>
-      <c r="AC4" s="5"/>
-      <c r="AD4" s="5"/>
-      <c r="AE4" s="5"/>
-      <c r="AF4" s="5"/>
-      <c r="AG4" s="5"/>
-      <c r="AH4" s="5"/>
+      <c r="D4" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" t="s">
+        <v>70</v>
+      </c>
+      <c r="M4" t="s">
+        <v>71</v>
+      </c>
+      <c r="N4" t="s">
+        <v>72</v>
+      </c>
+      <c r="O4" t="s">
+        <v>73</v>
+      </c>
+      <c r="P4" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>75</v>
+      </c>
+      <c r="R4" t="s">
+        <v>76</v>
+      </c>
+      <c r="S4" t="s">
+        <v>77</v>
+      </c>
+      <c r="T4" t="s">
+        <v>78</v>
+      </c>
+      <c r="U4" t="s">
+        <v>79</v>
+      </c>
+      <c r="V4" t="s">
+        <v>80</v>
+      </c>
+      <c r="W4" t="s">
+        <v>81</v>
+      </c>
+      <c r="X4" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>92</v>
+      </c>
       <c r="AI4" s="16" t="s">
         <v>13</v>
       </c>
@@ -1990,7 +2146,7 @@
       <c r="NI5" s="5"/>
     </row>
     <row r="6" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="46"/>
+      <c r="A6" s="43"/>
       <c r="B6" s="17">
         <v>2</v>
       </c>
@@ -2120,7 +2276,7 @@
       </c>
     </row>
     <row r="7" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="46"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="17">
         <v>3</v>
       </c>
@@ -2250,7 +2406,7 @@
       </c>
     </row>
     <row r="8" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="46"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="17">
         <v>4</v>
       </c>
@@ -2380,7 +2536,7 @@
       </c>
     </row>
     <row r="9" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="46"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="17">
         <v>5</v>
       </c>
@@ -2510,7 +2666,7 @@
       </c>
     </row>
     <row r="10" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="46"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="17">
         <v>6</v>
       </c>
@@ -2640,7 +2796,7 @@
       </c>
     </row>
     <row r="11" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="46"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="17">
         <v>7</v>
       </c>
@@ -2770,7 +2926,7 @@
       </c>
     </row>
     <row r="12" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="46"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="17">
         <v>8</v>
       </c>
@@ -2900,7 +3056,7 @@
       </c>
     </row>
     <row r="13" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="46"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="17">
         <v>9</v>
       </c>
@@ -3030,7 +3186,7 @@
       </c>
     </row>
     <row r="14" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="46"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="17">
         <v>10</v>
       </c>
@@ -3160,7 +3316,7 @@
       </c>
     </row>
     <row r="15" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="46"/>
+      <c r="A15" s="43"/>
       <c r="B15" s="17">
         <v>11</v>
       </c>
@@ -3290,7 +3446,7 @@
       </c>
     </row>
     <row r="16" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="46"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="17">
         <v>12</v>
       </c>
@@ -3420,7 +3576,7 @@
       </c>
     </row>
     <row r="17" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="46"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="17">
         <v>13</v>
       </c>
@@ -3550,7 +3706,7 @@
       </c>
     </row>
     <row r="18" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="46"/>
+      <c r="A18" s="43"/>
       <c r="B18" s="17">
         <v>14</v>
       </c>
@@ -3680,7 +3836,7 @@
       </c>
     </row>
     <row r="19" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="46"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="17">
         <v>15</v>
       </c>
@@ -3810,7 +3966,7 @@
       </c>
     </row>
     <row r="20" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="46"/>
+      <c r="A20" s="43"/>
       <c r="B20" s="17">
         <v>16</v>
       </c>
@@ -3940,7 +4096,7 @@
       </c>
     </row>
     <row r="21" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="46"/>
+      <c r="A21" s="43"/>
       <c r="B21" s="17">
         <v>17</v>
       </c>
@@ -4070,7 +4226,7 @@
       </c>
     </row>
     <row r="22" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="46"/>
+      <c r="A22" s="43"/>
       <c r="B22" s="17">
         <v>18</v>
       </c>
@@ -4200,7 +4356,7 @@
       </c>
     </row>
     <row r="23" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="46"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="17">
         <v>19</v>
       </c>
@@ -4330,7 +4486,7 @@
       </c>
     </row>
     <row r="24" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="46"/>
+      <c r="A24" s="43"/>
       <c r="B24" s="17">
         <v>20</v>
       </c>
@@ -4460,7 +4616,7 @@
       </c>
     </row>
     <row r="25" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="46"/>
+      <c r="A25" s="43"/>
       <c r="B25" s="17">
         <v>21</v>
       </c>
@@ -4590,7 +4746,7 @@
       </c>
     </row>
     <row r="26" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="46"/>
+      <c r="A26" s="43"/>
       <c r="B26" s="17">
         <v>22</v>
       </c>
@@ -4720,7 +4876,7 @@
       </c>
     </row>
     <row r="27" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="46"/>
+      <c r="A27" s="43"/>
       <c r="B27" s="17">
         <v>23</v>
       </c>
@@ -4850,7 +5006,7 @@
       </c>
     </row>
     <row r="28" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="46"/>
+      <c r="A28" s="43"/>
       <c r="B28" s="17">
         <v>24</v>
       </c>
@@ -4980,7 +5136,7 @@
       </c>
     </row>
     <row r="29" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="46"/>
+      <c r="A29" s="43"/>
       <c r="B29" s="17">
         <v>25</v>
       </c>
@@ -5110,7 +5266,7 @@
       </c>
     </row>
     <row r="30" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="46"/>
+      <c r="A30" s="43"/>
       <c r="B30" s="17">
         <v>26</v>
       </c>
@@ -5240,7 +5396,7 @@
       </c>
     </row>
     <row r="31" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="46"/>
+      <c r="A31" s="43"/>
       <c r="B31" s="17">
         <v>27</v>
       </c>
@@ -5370,7 +5526,7 @@
       </c>
     </row>
     <row r="32" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="46"/>
+      <c r="A32" s="43"/>
       <c r="B32" s="17">
         <v>28</v>
       </c>
@@ -5500,7 +5656,7 @@
       </c>
     </row>
     <row r="33" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="46"/>
+      <c r="A33" s="43"/>
       <c r="B33" s="17">
         <v>29</v>
       </c>
@@ -5630,7 +5786,7 @@
       </c>
     </row>
     <row r="34" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="46"/>
+      <c r="A34" s="43"/>
       <c r="B34" s="17">
         <v>30</v>
       </c>
@@ -5760,7 +5916,7 @@
       </c>
     </row>
     <row r="35" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="46"/>
+      <c r="A35" s="43"/>
       <c r="B35" s="17">
         <v>31</v>
       </c>
@@ -5890,7 +6046,7 @@
       </c>
     </row>
     <row r="36" spans="1:373" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="46"/>
+      <c r="A36" s="43"/>
       <c r="B36" s="21">
         <v>32</v>
       </c>
@@ -6349,7 +6505,7 @@
       <c r="NI36" s="5"/>
     </row>
     <row r="37" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="46"/>
+      <c r="A37" s="43"/>
       <c r="B37" s="17">
         <v>33</v>
       </c>
@@ -6478,7 +6634,7 @@
       </c>
     </row>
     <row r="38" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="46"/>
+      <c r="A38" s="43"/>
       <c r="B38" s="17">
         <v>34</v>
       </c>
@@ -6607,7 +6763,7 @@
       </c>
     </row>
     <row r="39" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="46"/>
+      <c r="A39" s="43"/>
       <c r="B39" s="17">
         <v>35</v>
       </c>
@@ -6736,7 +6892,7 @@
       </c>
     </row>
     <row r="40" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="46"/>
+      <c r="A40" s="43"/>
       <c r="B40" s="17">
         <v>36</v>
       </c>
@@ -6865,7 +7021,7 @@
       </c>
     </row>
     <row r="41" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="46"/>
+      <c r="A41" s="43"/>
       <c r="B41" s="17">
         <v>37</v>
       </c>
@@ -6994,7 +7150,7 @@
       </c>
     </row>
     <row r="42" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="46"/>
+      <c r="A42" s="43"/>
       <c r="B42" s="17">
         <v>38</v>
       </c>
@@ -7123,7 +7279,7 @@
       </c>
     </row>
     <row r="43" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="46"/>
+      <c r="A43" s="43"/>
       <c r="B43" s="17">
         <v>39</v>
       </c>
@@ -7252,7 +7408,7 @@
       </c>
     </row>
     <row r="44" spans="1:373" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="46"/>
+      <c r="A44" s="43"/>
       <c r="B44" s="17">
         <v>40</v>
       </c>
@@ -7711,7 +7867,7 @@
       <c r="NI44" s="5"/>
     </row>
     <row r="45" spans="1:373" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="43">
+      <c r="A45" s="44">
         <v>2</v>
       </c>
       <c r="B45" s="21">
@@ -8173,7 +8329,7 @@
       <c r="NI45" s="5"/>
     </row>
     <row r="46" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="44"/>
+      <c r="A46" s="45"/>
       <c r="B46" s="17">
         <v>2</v>
       </c>
@@ -8303,7 +8459,7 @@
       </c>
     </row>
     <row r="47" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="44"/>
+      <c r="A47" s="45"/>
       <c r="B47" s="17">
         <v>3</v>
       </c>
@@ -8433,7 +8589,7 @@
       </c>
     </row>
     <row r="48" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="44"/>
+      <c r="A48" s="45"/>
       <c r="B48" s="17">
         <v>4</v>
       </c>
@@ -8563,7 +8719,7 @@
       </c>
     </row>
     <row r="49" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="44"/>
+      <c r="A49" s="45"/>
       <c r="B49" s="17">
         <v>5</v>
       </c>
@@ -8693,7 +8849,7 @@
       </c>
     </row>
     <row r="50" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="44"/>
+      <c r="A50" s="45"/>
       <c r="B50" s="17">
         <v>6</v>
       </c>
@@ -8823,7 +8979,7 @@
       </c>
     </row>
     <row r="51" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="44"/>
+      <c r="A51" s="45"/>
       <c r="B51" s="17">
         <v>7</v>
       </c>
@@ -8953,7 +9109,7 @@
       </c>
     </row>
     <row r="52" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="44"/>
+      <c r="A52" s="45"/>
       <c r="B52" s="17">
         <v>8</v>
       </c>
@@ -9083,7 +9239,7 @@
       </c>
     </row>
     <row r="53" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="44"/>
+      <c r="A53" s="45"/>
       <c r="B53" s="17">
         <v>9</v>
       </c>
@@ -9213,7 +9369,7 @@
       </c>
     </row>
     <row r="54" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="44"/>
+      <c r="A54" s="45"/>
       <c r="B54" s="17">
         <v>10</v>
       </c>
@@ -9343,7 +9499,7 @@
       </c>
     </row>
     <row r="55" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="44"/>
+      <c r="A55" s="45"/>
       <c r="B55" s="17">
         <v>11</v>
       </c>
@@ -9473,7 +9629,7 @@
       </c>
     </row>
     <row r="56" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="44"/>
+      <c r="A56" s="45"/>
       <c r="B56" s="17">
         <v>12</v>
       </c>
@@ -9603,7 +9759,7 @@
       </c>
     </row>
     <row r="57" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="44"/>
+      <c r="A57" s="45"/>
       <c r="B57" s="17">
         <v>13</v>
       </c>
@@ -9733,7 +9889,7 @@
       </c>
     </row>
     <row r="58" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="44"/>
+      <c r="A58" s="45"/>
       <c r="B58" s="17">
         <v>14</v>
       </c>
@@ -9863,7 +10019,7 @@
       </c>
     </row>
     <row r="59" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="44"/>
+      <c r="A59" s="45"/>
       <c r="B59" s="17">
         <v>15</v>
       </c>
@@ -9993,7 +10149,7 @@
       </c>
     </row>
     <row r="60" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="44"/>
+      <c r="A60" s="45"/>
       <c r="B60" s="17">
         <v>16</v>
       </c>
@@ -10123,7 +10279,7 @@
       </c>
     </row>
     <row r="61" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="44"/>
+      <c r="A61" s="45"/>
       <c r="B61" s="17">
         <v>17</v>
       </c>
@@ -10253,7 +10409,7 @@
       </c>
     </row>
     <row r="62" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="44"/>
+      <c r="A62" s="45"/>
       <c r="B62" s="17">
         <v>18</v>
       </c>
@@ -10383,7 +10539,7 @@
       </c>
     </row>
     <row r="63" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="44"/>
+      <c r="A63" s="45"/>
       <c r="B63" s="17">
         <v>19</v>
       </c>
@@ -10513,7 +10669,7 @@
       </c>
     </row>
     <row r="64" spans="1:43" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="44"/>
+      <c r="A64" s="45"/>
       <c r="B64" s="17">
         <v>20</v>
       </c>
@@ -10643,7 +10799,7 @@
       </c>
     </row>
     <row r="65" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="44"/>
+      <c r="A65" s="45"/>
       <c r="B65" s="17">
         <v>21</v>
       </c>
@@ -10773,7 +10929,7 @@
       </c>
     </row>
     <row r="66" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="44"/>
+      <c r="A66" s="45"/>
       <c r="B66" s="17">
         <v>22</v>
       </c>
@@ -10903,7 +11059,7 @@
       </c>
     </row>
     <row r="67" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="44"/>
+      <c r="A67" s="45"/>
       <c r="B67" s="17">
         <v>23</v>
       </c>
@@ -11033,7 +11189,7 @@
       </c>
     </row>
     <row r="68" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="44"/>
+      <c r="A68" s="45"/>
       <c r="B68" s="17">
         <v>24</v>
       </c>
@@ -11163,7 +11319,7 @@
       </c>
     </row>
     <row r="69" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="44"/>
+      <c r="A69" s="45"/>
       <c r="B69" s="17">
         <v>25</v>
       </c>
@@ -11293,7 +11449,7 @@
       </c>
     </row>
     <row r="70" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="44"/>
+      <c r="A70" s="45"/>
       <c r="B70" s="17">
         <v>26</v>
       </c>
@@ -11423,7 +11579,7 @@
       </c>
     </row>
     <row r="71" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="44"/>
+      <c r="A71" s="45"/>
       <c r="B71" s="17">
         <v>27</v>
       </c>
@@ -11553,7 +11709,7 @@
       </c>
     </row>
     <row r="72" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="44"/>
+      <c r="A72" s="45"/>
       <c r="B72" s="17">
         <v>28</v>
       </c>
@@ -11683,7 +11839,7 @@
       </c>
     </row>
     <row r="73" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="44"/>
+      <c r="A73" s="45"/>
       <c r="B73" s="17">
         <v>29</v>
       </c>
@@ -11813,7 +11969,7 @@
       </c>
     </row>
     <row r="74" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="44"/>
+      <c r="A74" s="45"/>
       <c r="B74" s="17">
         <v>30</v>
       </c>
@@ -11943,7 +12099,7 @@
       </c>
     </row>
     <row r="75" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="44"/>
+      <c r="A75" s="45"/>
       <c r="B75" s="17">
         <v>31</v>
       </c>
@@ -12073,7 +12229,7 @@
       </c>
     </row>
     <row r="76" spans="1:373" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="44"/>
+      <c r="A76" s="45"/>
       <c r="B76" s="21">
         <v>32</v>
       </c>
@@ -12532,7 +12688,7 @@
       <c r="NI76" s="5"/>
     </row>
     <row r="77" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="44"/>
+      <c r="A77" s="45"/>
       <c r="B77" s="17">
         <v>33</v>
       </c>
@@ -12661,7 +12817,7 @@
       </c>
     </row>
     <row r="78" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="44"/>
+      <c r="A78" s="45"/>
       <c r="B78" s="17">
         <v>34</v>
       </c>
@@ -12790,7 +12946,7 @@
       </c>
     </row>
     <row r="79" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="44"/>
+      <c r="A79" s="45"/>
       <c r="B79" s="17">
         <v>35</v>
       </c>
@@ -12919,7 +13075,7 @@
       </c>
     </row>
     <row r="80" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="44"/>
+      <c r="A80" s="45"/>
       <c r="B80" s="17">
         <v>36</v>
       </c>
@@ -13048,7 +13204,7 @@
       </c>
     </row>
     <row r="81" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="44"/>
+      <c r="A81" s="45"/>
       <c r="B81" s="17">
         <v>37</v>
       </c>
@@ -13177,7 +13333,7 @@
       </c>
     </row>
     <row r="82" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="44"/>
+      <c r="A82" s="45"/>
       <c r="B82" s="17">
         <v>38</v>
       </c>
@@ -13306,7 +13462,7 @@
       </c>
     </row>
     <row r="83" spans="1:373" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="44"/>
+      <c r="A83" s="45"/>
       <c r="B83" s="17">
         <v>39</v>
       </c>
@@ -13435,7 +13591,7 @@
       </c>
     </row>
     <row r="84" spans="1:373" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="45"/>
+      <c r="A84" s="46"/>
       <c r="B84" s="27">
         <v>40</v>
       </c>
@@ -13894,7 +14050,7 @@
       <c r="NI84" s="5"/>
     </row>
     <row r="85" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A85" s="46">
+      <c r="A85" s="43">
         <v>3</v>
       </c>
       <c r="B85" s="17">
@@ -14026,7 +14182,7 @@
       </c>
     </row>
     <row r="86" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A86" s="46"/>
+      <c r="A86" s="43"/>
       <c r="B86" s="17">
         <v>2</v>
       </c>
@@ -14156,7 +14312,7 @@
       </c>
     </row>
     <row r="87" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A87" s="46"/>
+      <c r="A87" s="43"/>
       <c r="B87" s="17">
         <v>3</v>
       </c>
@@ -14286,7 +14442,7 @@
       </c>
     </row>
     <row r="88" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A88" s="46"/>
+      <c r="A88" s="43"/>
       <c r="B88" s="17">
         <v>4</v>
       </c>
@@ -14416,7 +14572,7 @@
       </c>
     </row>
     <row r="89" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A89" s="46"/>
+      <c r="A89" s="43"/>
       <c r="B89" s="17">
         <v>5</v>
       </c>
@@ -14546,7 +14702,7 @@
       </c>
     </row>
     <row r="90" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A90" s="46"/>
+      <c r="A90" s="43"/>
       <c r="B90" s="17">
         <v>6</v>
       </c>
@@ -14676,7 +14832,7 @@
       </c>
     </row>
     <row r="91" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A91" s="46"/>
+      <c r="A91" s="43"/>
       <c r="B91" s="17">
         <v>7</v>
       </c>
@@ -14806,7 +14962,7 @@
       </c>
     </row>
     <row r="92" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A92" s="46"/>
+      <c r="A92" s="43"/>
       <c r="B92" s="17">
         <v>8</v>
       </c>
@@ -14936,7 +15092,7 @@
       </c>
     </row>
     <row r="93" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A93" s="46"/>
+      <c r="A93" s="43"/>
       <c r="B93" s="17">
         <v>9</v>
       </c>
@@ -15066,7 +15222,7 @@
       </c>
     </row>
     <row r="94" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A94" s="46"/>
+      <c r="A94" s="43"/>
       <c r="B94" s="17">
         <v>10</v>
       </c>
@@ -15196,7 +15352,7 @@
       </c>
     </row>
     <row r="95" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A95" s="46"/>
+      <c r="A95" s="43"/>
       <c r="B95" s="17">
         <v>11</v>
       </c>
@@ -15326,7 +15482,7 @@
       </c>
     </row>
     <row r="96" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A96" s="46"/>
+      <c r="A96" s="43"/>
       <c r="B96" s="17">
         <v>12</v>
       </c>
@@ -15456,7 +15612,7 @@
       </c>
     </row>
     <row r="97" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A97" s="46"/>
+      <c r="A97" s="43"/>
       <c r="B97" s="17">
         <v>13</v>
       </c>
@@ -15586,7 +15742,7 @@
       </c>
     </row>
     <row r="98" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A98" s="46"/>
+      <c r="A98" s="43"/>
       <c r="B98" s="17">
         <v>14</v>
       </c>
@@ -15716,7 +15872,7 @@
       </c>
     </row>
     <row r="99" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A99" s="46"/>
+      <c r="A99" s="43"/>
       <c r="B99" s="17">
         <v>15</v>
       </c>
@@ -15846,7 +16002,7 @@
       </c>
     </row>
     <row r="100" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A100" s="46"/>
+      <c r="A100" s="43"/>
       <c r="B100" s="17">
         <v>16</v>
       </c>
@@ -15976,7 +16132,7 @@
       </c>
     </row>
     <row r="101" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A101" s="46"/>
+      <c r="A101" s="43"/>
       <c r="B101" s="17">
         <v>17</v>
       </c>
@@ -16106,7 +16262,7 @@
       </c>
     </row>
     <row r="102" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A102" s="46"/>
+      <c r="A102" s="43"/>
       <c r="B102" s="17">
         <v>18</v>
       </c>
@@ -16236,7 +16392,7 @@
       </c>
     </row>
     <row r="103" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A103" s="46"/>
+      <c r="A103" s="43"/>
       <c r="B103" s="17">
         <v>19</v>
       </c>
@@ -16366,7 +16522,7 @@
       </c>
     </row>
     <row r="104" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A104" s="46"/>
+      <c r="A104" s="43"/>
       <c r="B104" s="17">
         <v>20</v>
       </c>
@@ -16496,7 +16652,7 @@
       </c>
     </row>
     <row r="105" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A105" s="46"/>
+      <c r="A105" s="43"/>
       <c r="B105" s="17">
         <v>21</v>
       </c>
@@ -16626,7 +16782,7 @@
       </c>
     </row>
     <row r="106" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A106" s="46"/>
+      <c r="A106" s="43"/>
       <c r="B106" s="17">
         <v>22</v>
       </c>
@@ -16756,7 +16912,7 @@
       </c>
     </row>
     <row r="107" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A107" s="46"/>
+      <c r="A107" s="43"/>
       <c r="B107" s="17">
         <v>23</v>
       </c>
@@ -16886,7 +17042,7 @@
       </c>
     </row>
     <row r="108" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A108" s="46"/>
+      <c r="A108" s="43"/>
       <c r="B108" s="17">
         <v>24</v>
       </c>
@@ -17016,7 +17172,7 @@
       </c>
     </row>
     <row r="109" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A109" s="46"/>
+      <c r="A109" s="43"/>
       <c r="B109" s="17">
         <v>25</v>
       </c>
@@ -17146,7 +17302,7 @@
       </c>
     </row>
     <row r="110" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A110" s="46"/>
+      <c r="A110" s="43"/>
       <c r="B110" s="17">
         <v>26</v>
       </c>
@@ -17276,7 +17432,7 @@
       </c>
     </row>
     <row r="111" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A111" s="46"/>
+      <c r="A111" s="43"/>
       <c r="B111" s="17">
         <v>27</v>
       </c>
@@ -17406,7 +17562,7 @@
       </c>
     </row>
     <row r="112" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A112" s="46"/>
+      <c r="A112" s="43"/>
       <c r="B112" s="17">
         <v>28</v>
       </c>
@@ -17536,7 +17692,7 @@
       </c>
     </row>
     <row r="113" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A113" s="46"/>
+      <c r="A113" s="43"/>
       <c r="B113" s="17">
         <v>29</v>
       </c>
@@ -17666,7 +17822,7 @@
       </c>
     </row>
     <row r="114" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A114" s="46"/>
+      <c r="A114" s="43"/>
       <c r="B114" s="17">
         <v>30</v>
       </c>
@@ -17796,7 +17952,7 @@
       </c>
     </row>
     <row r="115" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A115" s="46"/>
+      <c r="A115" s="43"/>
       <c r="B115" s="17">
         <v>31</v>
       </c>
@@ -17926,7 +18082,7 @@
       </c>
     </row>
     <row r="116" spans="1:373" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="46"/>
+      <c r="A116" s="43"/>
       <c r="B116" s="21">
         <v>32</v>
       </c>
@@ -18385,7 +18541,7 @@
       <c r="NI116" s="5"/>
     </row>
     <row r="117" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A117" s="46"/>
+      <c r="A117" s="43"/>
       <c r="B117" s="17">
         <v>33</v>
       </c>
@@ -18514,7 +18670,7 @@
       </c>
     </row>
     <row r="118" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A118" s="46"/>
+      <c r="A118" s="43"/>
       <c r="B118" s="17">
         <v>34</v>
       </c>
@@ -18643,7 +18799,7 @@
       </c>
     </row>
     <row r="119" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A119" s="46"/>
+      <c r="A119" s="43"/>
       <c r="B119" s="17">
         <v>35</v>
       </c>
@@ -18772,7 +18928,7 @@
       </c>
     </row>
     <row r="120" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A120" s="46"/>
+      <c r="A120" s="43"/>
       <c r="B120" s="17">
         <v>36</v>
       </c>
@@ -18901,7 +19057,7 @@
       </c>
     </row>
     <row r="121" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A121" s="46"/>
+      <c r="A121" s="43"/>
       <c r="B121" s="17">
         <v>37</v>
       </c>
@@ -19030,7 +19186,7 @@
       </c>
     </row>
     <row r="122" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A122" s="46"/>
+      <c r="A122" s="43"/>
       <c r="B122" s="17">
         <v>38</v>
       </c>
@@ -19159,7 +19315,7 @@
       </c>
     </row>
     <row r="123" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A123" s="46"/>
+      <c r="A123" s="43"/>
       <c r="B123" s="17">
         <v>39</v>
       </c>
@@ -19288,7 +19444,7 @@
       </c>
     </row>
     <row r="124" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A124" s="46"/>
+      <c r="A124" s="43"/>
       <c r="B124" s="17">
         <v>40</v>
       </c>
@@ -19417,7 +19573,7 @@
       </c>
     </row>
     <row r="125" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A125" s="43">
+      <c r="A125" s="44">
         <v>4</v>
       </c>
       <c r="B125" s="21">
@@ -19549,7 +19705,7 @@
       </c>
     </row>
     <row r="126" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A126" s="44"/>
+      <c r="A126" s="45"/>
       <c r="B126" s="17">
         <v>2</v>
       </c>
@@ -19679,7 +19835,7 @@
       </c>
     </row>
     <row r="127" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A127" s="44"/>
+      <c r="A127" s="45"/>
       <c r="B127" s="17">
         <v>3</v>
       </c>
@@ -19809,7 +19965,7 @@
       </c>
     </row>
     <row r="128" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A128" s="44"/>
+      <c r="A128" s="45"/>
       <c r="B128" s="17">
         <v>4</v>
       </c>
@@ -19939,7 +20095,7 @@
       </c>
     </row>
     <row r="129" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A129" s="44"/>
+      <c r="A129" s="45"/>
       <c r="B129" s="17">
         <v>5</v>
       </c>
@@ -20069,7 +20225,7 @@
       </c>
     </row>
     <row r="130" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A130" s="44"/>
+      <c r="A130" s="45"/>
       <c r="B130" s="17">
         <v>6</v>
       </c>
@@ -20199,7 +20355,7 @@
       </c>
     </row>
     <row r="131" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A131" s="44"/>
+      <c r="A131" s="45"/>
       <c r="B131" s="17">
         <v>7</v>
       </c>
@@ -20329,7 +20485,7 @@
       </c>
     </row>
     <row r="132" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A132" s="44"/>
+      <c r="A132" s="45"/>
       <c r="B132" s="17">
         <v>8</v>
       </c>
@@ -20459,7 +20615,7 @@
       </c>
     </row>
     <row r="133" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A133" s="44"/>
+      <c r="A133" s="45"/>
       <c r="B133" s="17">
         <v>9</v>
       </c>
@@ -20589,7 +20745,7 @@
       </c>
     </row>
     <row r="134" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A134" s="44"/>
+      <c r="A134" s="45"/>
       <c r="B134" s="17">
         <v>10</v>
       </c>
@@ -20719,7 +20875,7 @@
       </c>
     </row>
     <row r="135" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A135" s="44"/>
+      <c r="A135" s="45"/>
       <c r="B135" s="17">
         <v>11</v>
       </c>
@@ -20849,7 +21005,7 @@
       </c>
     </row>
     <row r="136" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A136" s="44"/>
+      <c r="A136" s="45"/>
       <c r="B136" s="17">
         <v>12</v>
       </c>
@@ -20979,7 +21135,7 @@
       </c>
     </row>
     <row r="137" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A137" s="44"/>
+      <c r="A137" s="45"/>
       <c r="B137" s="17">
         <v>13</v>
       </c>
@@ -21109,7 +21265,7 @@
       </c>
     </row>
     <row r="138" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A138" s="44"/>
+      <c r="A138" s="45"/>
       <c r="B138" s="17">
         <v>14</v>
       </c>
@@ -21239,7 +21395,7 @@
       </c>
     </row>
     <row r="139" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A139" s="44"/>
+      <c r="A139" s="45"/>
       <c r="B139" s="17">
         <v>15</v>
       </c>
@@ -21369,7 +21525,7 @@
       </c>
     </row>
     <row r="140" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A140" s="44"/>
+      <c r="A140" s="45"/>
       <c r="B140" s="17">
         <v>16</v>
       </c>
@@ -21499,7 +21655,7 @@
       </c>
     </row>
     <row r="141" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A141" s="44"/>
+      <c r="A141" s="45"/>
       <c r="B141" s="17">
         <v>17</v>
       </c>
@@ -21629,7 +21785,7 @@
       </c>
     </row>
     <row r="142" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A142" s="44"/>
+      <c r="A142" s="45"/>
       <c r="B142" s="17">
         <v>18</v>
       </c>
@@ -21759,7 +21915,7 @@
       </c>
     </row>
     <row r="143" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A143" s="44"/>
+      <c r="A143" s="45"/>
       <c r="B143" s="17">
         <v>19</v>
       </c>
@@ -21889,7 +22045,7 @@
       </c>
     </row>
     <row r="144" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A144" s="44"/>
+      <c r="A144" s="45"/>
       <c r="B144" s="17">
         <v>20</v>
       </c>
@@ -22019,7 +22175,7 @@
       </c>
     </row>
     <row r="145" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A145" s="44"/>
+      <c r="A145" s="45"/>
       <c r="B145" s="17">
         <v>21</v>
       </c>
@@ -22149,7 +22305,7 @@
       </c>
     </row>
     <row r="146" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A146" s="44"/>
+      <c r="A146" s="45"/>
       <c r="B146" s="17">
         <v>22</v>
       </c>
@@ -22279,7 +22435,7 @@
       </c>
     </row>
     <row r="147" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A147" s="44"/>
+      <c r="A147" s="45"/>
       <c r="B147" s="17">
         <v>23</v>
       </c>
@@ -22409,7 +22565,7 @@
       </c>
     </row>
     <row r="148" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A148" s="44"/>
+      <c r="A148" s="45"/>
       <c r="B148" s="17">
         <v>24</v>
       </c>
@@ -22539,7 +22695,7 @@
       </c>
     </row>
     <row r="149" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A149" s="44"/>
+      <c r="A149" s="45"/>
       <c r="B149" s="17">
         <v>25</v>
       </c>
@@ -22669,7 +22825,7 @@
       </c>
     </row>
     <row r="150" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A150" s="44"/>
+      <c r="A150" s="45"/>
       <c r="B150" s="17">
         <v>26</v>
       </c>
@@ -22799,7 +22955,7 @@
       </c>
     </row>
     <row r="151" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A151" s="44"/>
+      <c r="A151" s="45"/>
       <c r="B151" s="17">
         <v>27</v>
       </c>
@@ -22929,7 +23085,7 @@
       </c>
     </row>
     <row r="152" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A152" s="44"/>
+      <c r="A152" s="45"/>
       <c r="B152" s="17">
         <v>28</v>
       </c>
@@ -23059,7 +23215,7 @@
       </c>
     </row>
     <row r="153" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A153" s="44"/>
+      <c r="A153" s="45"/>
       <c r="B153" s="17">
         <v>29</v>
       </c>
@@ -23189,7 +23345,7 @@
       </c>
     </row>
     <row r="154" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A154" s="44"/>
+      <c r="A154" s="45"/>
       <c r="B154" s="17">
         <v>30</v>
       </c>
@@ -23319,7 +23475,7 @@
       </c>
     </row>
     <row r="155" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A155" s="44"/>
+      <c r="A155" s="45"/>
       <c r="B155" s="17">
         <v>31</v>
       </c>
@@ -23449,7 +23605,7 @@
       </c>
     </row>
     <row r="156" spans="1:373" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A156" s="44"/>
+      <c r="A156" s="45"/>
       <c r="B156" s="21">
         <v>32</v>
       </c>
@@ -23908,7 +24064,7 @@
       <c r="NI156" s="5"/>
     </row>
     <row r="157" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A157" s="44"/>
+      <c r="A157" s="45"/>
       <c r="B157" s="17">
         <v>33</v>
       </c>
@@ -24037,7 +24193,7 @@
       </c>
     </row>
     <row r="158" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A158" s="44"/>
+      <c r="A158" s="45"/>
       <c r="B158" s="17">
         <v>34</v>
       </c>
@@ -24166,7 +24322,7 @@
       </c>
     </row>
     <row r="159" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A159" s="44"/>
+      <c r="A159" s="45"/>
       <c r="B159" s="17">
         <v>35</v>
       </c>
@@ -24295,7 +24451,7 @@
       </c>
     </row>
     <row r="160" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A160" s="44"/>
+      <c r="A160" s="45"/>
       <c r="B160" s="17">
         <v>36</v>
       </c>
@@ -24424,7 +24580,7 @@
       </c>
     </row>
     <row r="161" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A161" s="44"/>
+      <c r="A161" s="45"/>
       <c r="B161" s="17">
         <v>37</v>
       </c>
@@ -24553,7 +24709,7 @@
       </c>
     </row>
     <row r="162" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A162" s="44"/>
+      <c r="A162" s="45"/>
       <c r="B162" s="17">
         <v>38</v>
       </c>
@@ -24682,7 +24838,7 @@
       </c>
     </row>
     <row r="163" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A163" s="44"/>
+      <c r="A163" s="45"/>
       <c r="B163" s="17">
         <v>39</v>
       </c>
@@ -24811,7 +24967,7 @@
       </c>
     </row>
     <row r="164" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A164" s="45"/>
+      <c r="A164" s="46"/>
       <c r="B164" s="27">
         <v>40</v>
       </c>
@@ -24940,7 +25096,7 @@
       </c>
     </row>
     <row r="165" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A165" s="46">
+      <c r="A165" s="43">
         <v>5</v>
       </c>
       <c r="B165" s="17">
@@ -25072,7 +25228,7 @@
       </c>
     </row>
     <row r="166" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A166" s="46"/>
+      <c r="A166" s="43"/>
       <c r="B166" s="17">
         <v>2</v>
       </c>
@@ -25202,7 +25358,7 @@
       </c>
     </row>
     <row r="167" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A167" s="46"/>
+      <c r="A167" s="43"/>
       <c r="B167" s="17">
         <v>3</v>
       </c>
@@ -25332,7 +25488,7 @@
       </c>
     </row>
     <row r="168" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A168" s="46"/>
+      <c r="A168" s="43"/>
       <c r="B168" s="17">
         <v>4</v>
       </c>
@@ -25462,7 +25618,7 @@
       </c>
     </row>
     <row r="169" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A169" s="46"/>
+      <c r="A169" s="43"/>
       <c r="B169" s="17">
         <v>5</v>
       </c>
@@ -25592,7 +25748,7 @@
       </c>
     </row>
     <row r="170" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A170" s="46"/>
+      <c r="A170" s="43"/>
       <c r="B170" s="17">
         <v>6</v>
       </c>
@@ -25722,7 +25878,7 @@
       </c>
     </row>
     <row r="171" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A171" s="46"/>
+      <c r="A171" s="43"/>
       <c r="B171" s="17">
         <v>7</v>
       </c>
@@ -25852,7 +26008,7 @@
       </c>
     </row>
     <row r="172" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A172" s="46"/>
+      <c r="A172" s="43"/>
       <c r="B172" s="17">
         <v>8</v>
       </c>
@@ -25982,7 +26138,7 @@
       </c>
     </row>
     <row r="173" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A173" s="46"/>
+      <c r="A173" s="43"/>
       <c r="B173" s="17">
         <v>9</v>
       </c>
@@ -26112,7 +26268,7 @@
       </c>
     </row>
     <row r="174" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A174" s="46"/>
+      <c r="A174" s="43"/>
       <c r="B174" s="17">
         <v>10</v>
       </c>
@@ -26242,7 +26398,7 @@
       </c>
     </row>
     <row r="175" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A175" s="46"/>
+      <c r="A175" s="43"/>
       <c r="B175" s="17">
         <v>11</v>
       </c>
@@ -26372,7 +26528,7 @@
       </c>
     </row>
     <row r="176" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A176" s="46"/>
+      <c r="A176" s="43"/>
       <c r="B176" s="17">
         <v>12</v>
       </c>
@@ -26502,7 +26658,7 @@
       </c>
     </row>
     <row r="177" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A177" s="46"/>
+      <c r="A177" s="43"/>
       <c r="B177" s="17">
         <v>13</v>
       </c>
@@ -26632,7 +26788,7 @@
       </c>
     </row>
     <row r="178" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A178" s="46"/>
+      <c r="A178" s="43"/>
       <c r="B178" s="17">
         <v>14</v>
       </c>
@@ -26762,7 +26918,7 @@
       </c>
     </row>
     <row r="179" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A179" s="46"/>
+      <c r="A179" s="43"/>
       <c r="B179" s="17">
         <v>15</v>
       </c>
@@ -26892,7 +27048,7 @@
       </c>
     </row>
     <row r="180" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A180" s="46"/>
+      <c r="A180" s="43"/>
       <c r="B180" s="17">
         <v>16</v>
       </c>
@@ -27022,7 +27178,7 @@
       </c>
     </row>
     <row r="181" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A181" s="46"/>
+      <c r="A181" s="43"/>
       <c r="B181" s="17">
         <v>17</v>
       </c>
@@ -27152,7 +27308,7 @@
       </c>
     </row>
     <row r="182" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A182" s="46"/>
+      <c r="A182" s="43"/>
       <c r="B182" s="17">
         <v>18</v>
       </c>
@@ -27282,7 +27438,7 @@
       </c>
     </row>
     <row r="183" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A183" s="46"/>
+      <c r="A183" s="43"/>
       <c r="B183" s="17">
         <v>19</v>
       </c>
@@ -27412,7 +27568,7 @@
       </c>
     </row>
     <row r="184" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A184" s="46"/>
+      <c r="A184" s="43"/>
       <c r="B184" s="17">
         <v>20</v>
       </c>
@@ -27542,7 +27698,7 @@
       </c>
     </row>
     <row r="185" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A185" s="46"/>
+      <c r="A185" s="43"/>
       <c r="B185" s="17">
         <v>21</v>
       </c>
@@ -27672,7 +27828,7 @@
       </c>
     </row>
     <row r="186" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A186" s="46"/>
+      <c r="A186" s="43"/>
       <c r="B186" s="17">
         <v>22</v>
       </c>
@@ -27802,7 +27958,7 @@
       </c>
     </row>
     <row r="187" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A187" s="46"/>
+      <c r="A187" s="43"/>
       <c r="B187" s="17">
         <v>23</v>
       </c>
@@ -27932,7 +28088,7 @@
       </c>
     </row>
     <row r="188" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A188" s="46"/>
+      <c r="A188" s="43"/>
       <c r="B188" s="17">
         <v>24</v>
       </c>
@@ -28062,7 +28218,7 @@
       </c>
     </row>
     <row r="189" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A189" s="46"/>
+      <c r="A189" s="43"/>
       <c r="B189" s="17">
         <v>25</v>
       </c>
@@ -28192,7 +28348,7 @@
       </c>
     </row>
     <row r="190" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A190" s="46"/>
+      <c r="A190" s="43"/>
       <c r="B190" s="17">
         <v>26</v>
       </c>
@@ -28322,7 +28478,7 @@
       </c>
     </row>
     <row r="191" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A191" s="46"/>
+      <c r="A191" s="43"/>
       <c r="B191" s="17">
         <v>27</v>
       </c>
@@ -28452,7 +28608,7 @@
       </c>
     </row>
     <row r="192" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A192" s="46"/>
+      <c r="A192" s="43"/>
       <c r="B192" s="17">
         <v>28</v>
       </c>
@@ -28582,7 +28738,7 @@
       </c>
     </row>
     <row r="193" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A193" s="46"/>
+      <c r="A193" s="43"/>
       <c r="B193" s="17">
         <v>29</v>
       </c>
@@ -28712,7 +28868,7 @@
       </c>
     </row>
     <row r="194" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A194" s="46"/>
+      <c r="A194" s="43"/>
       <c r="B194" s="17">
         <v>30</v>
       </c>
@@ -28842,7 +28998,7 @@
       </c>
     </row>
     <row r="195" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A195" s="46"/>
+      <c r="A195" s="43"/>
       <c r="B195" s="17">
         <v>31</v>
       </c>
@@ -28972,7 +29128,7 @@
       </c>
     </row>
     <row r="196" spans="1:373" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A196" s="46"/>
+      <c r="A196" s="43"/>
       <c r="B196" s="21">
         <v>32</v>
       </c>
@@ -29431,7 +29587,7 @@
       <c r="NI196" s="5"/>
     </row>
     <row r="197" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A197" s="46"/>
+      <c r="A197" s="43"/>
       <c r="B197" s="17">
         <v>33</v>
       </c>
@@ -29560,7 +29716,7 @@
       </c>
     </row>
     <row r="198" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A198" s="46"/>
+      <c r="A198" s="43"/>
       <c r="B198" s="17">
         <v>34</v>
       </c>
@@ -29689,7 +29845,7 @@
       </c>
     </row>
     <row r="199" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A199" s="46"/>
+      <c r="A199" s="43"/>
       <c r="B199" s="17">
         <v>35</v>
       </c>
@@ -29818,7 +29974,7 @@
       </c>
     </row>
     <row r="200" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A200" s="46"/>
+      <c r="A200" s="43"/>
       <c r="B200" s="17">
         <v>36</v>
       </c>
@@ -29947,7 +30103,7 @@
       </c>
     </row>
     <row r="201" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A201" s="46"/>
+      <c r="A201" s="43"/>
       <c r="B201" s="17">
         <v>37</v>
       </c>
@@ -30076,7 +30232,7 @@
       </c>
     </row>
     <row r="202" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A202" s="46"/>
+      <c r="A202" s="43"/>
       <c r="B202" s="17">
         <v>38</v>
       </c>
@@ -30205,7 +30361,7 @@
       </c>
     </row>
     <row r="203" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A203" s="46"/>
+      <c r="A203" s="43"/>
       <c r="B203" s="17">
         <v>39</v>
       </c>
@@ -30334,7 +30490,7 @@
       </c>
     </row>
     <row r="204" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A204" s="46"/>
+      <c r="A204" s="43"/>
       <c r="B204" s="17">
         <v>40</v>
       </c>
@@ -30463,7 +30619,7 @@
       </c>
     </row>
     <row r="205" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A205" s="43">
+      <c r="A205" s="44">
         <v>6</v>
       </c>
       <c r="B205" s="21">
@@ -30595,7 +30751,7 @@
       </c>
     </row>
     <row r="206" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A206" s="44"/>
+      <c r="A206" s="45"/>
       <c r="B206" s="17">
         <v>2</v>
       </c>
@@ -30725,7 +30881,7 @@
       </c>
     </row>
     <row r="207" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A207" s="44"/>
+      <c r="A207" s="45"/>
       <c r="B207" s="17">
         <v>3</v>
       </c>
@@ -30855,7 +31011,7 @@
       </c>
     </row>
     <row r="208" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A208" s="44"/>
+      <c r="A208" s="45"/>
       <c r="B208" s="17">
         <v>4</v>
       </c>
@@ -30985,7 +31141,7 @@
       </c>
     </row>
     <row r="209" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A209" s="44"/>
+      <c r="A209" s="45"/>
       <c r="B209" s="17">
         <v>5</v>
       </c>
@@ -31115,7 +31271,7 @@
       </c>
     </row>
     <row r="210" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A210" s="44"/>
+      <c r="A210" s="45"/>
       <c r="B210" s="17">
         <v>6</v>
       </c>
@@ -31245,7 +31401,7 @@
       </c>
     </row>
     <row r="211" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A211" s="44"/>
+      <c r="A211" s="45"/>
       <c r="B211" s="17">
         <v>7</v>
       </c>
@@ -31375,7 +31531,7 @@
       </c>
     </row>
     <row r="212" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A212" s="44"/>
+      <c r="A212" s="45"/>
       <c r="B212" s="17">
         <v>8</v>
       </c>
@@ -31505,7 +31661,7 @@
       </c>
     </row>
     <row r="213" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A213" s="44"/>
+      <c r="A213" s="45"/>
       <c r="B213" s="17">
         <v>9</v>
       </c>
@@ -31635,7 +31791,7 @@
       </c>
     </row>
     <row r="214" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A214" s="44"/>
+      <c r="A214" s="45"/>
       <c r="B214" s="17">
         <v>10</v>
       </c>
@@ -31765,7 +31921,7 @@
       </c>
     </row>
     <row r="215" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A215" s="44"/>
+      <c r="A215" s="45"/>
       <c r="B215" s="17">
         <v>11</v>
       </c>
@@ -31895,7 +32051,7 @@
       </c>
     </row>
     <row r="216" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A216" s="44"/>
+      <c r="A216" s="45"/>
       <c r="B216" s="17">
         <v>12</v>
       </c>
@@ -32025,7 +32181,7 @@
       </c>
     </row>
     <row r="217" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A217" s="44"/>
+      <c r="A217" s="45"/>
       <c r="B217" s="17">
         <v>13</v>
       </c>
@@ -32155,7 +32311,7 @@
       </c>
     </row>
     <row r="218" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A218" s="44"/>
+      <c r="A218" s="45"/>
       <c r="B218" s="17">
         <v>14</v>
       </c>
@@ -32285,7 +32441,7 @@
       </c>
     </row>
     <row r="219" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A219" s="44"/>
+      <c r="A219" s="45"/>
       <c r="B219" s="17">
         <v>15</v>
       </c>
@@ -32415,7 +32571,7 @@
       </c>
     </row>
     <row r="220" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A220" s="44"/>
+      <c r="A220" s="45"/>
       <c r="B220" s="17">
         <v>16</v>
       </c>
@@ -32545,7 +32701,7 @@
       </c>
     </row>
     <row r="221" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A221" s="44"/>
+      <c r="A221" s="45"/>
       <c r="B221" s="17">
         <v>17</v>
       </c>
@@ -32675,7 +32831,7 @@
       </c>
     </row>
     <row r="222" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A222" s="44"/>
+      <c r="A222" s="45"/>
       <c r="B222" s="17">
         <v>18</v>
       </c>
@@ -32805,7 +32961,7 @@
       </c>
     </row>
     <row r="223" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A223" s="44"/>
+      <c r="A223" s="45"/>
       <c r="B223" s="17">
         <v>19</v>
       </c>
@@ -32935,7 +33091,7 @@
       </c>
     </row>
     <row r="224" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A224" s="44"/>
+      <c r="A224" s="45"/>
       <c r="B224" s="17">
         <v>20</v>
       </c>
@@ -33065,7 +33221,7 @@
       </c>
     </row>
     <row r="225" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A225" s="44"/>
+      <c r="A225" s="45"/>
       <c r="B225" s="17">
         <v>21</v>
       </c>
@@ -33195,7 +33351,7 @@
       </c>
     </row>
     <row r="226" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A226" s="44"/>
+      <c r="A226" s="45"/>
       <c r="B226" s="17">
         <v>22</v>
       </c>
@@ -33325,7 +33481,7 @@
       </c>
     </row>
     <row r="227" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A227" s="44"/>
+      <c r="A227" s="45"/>
       <c r="B227" s="17">
         <v>23</v>
       </c>
@@ -33455,7 +33611,7 @@
       </c>
     </row>
     <row r="228" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A228" s="44"/>
+      <c r="A228" s="45"/>
       <c r="B228" s="17">
         <v>24</v>
       </c>
@@ -33585,7 +33741,7 @@
       </c>
     </row>
     <row r="229" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A229" s="44"/>
+      <c r="A229" s="45"/>
       <c r="B229" s="17">
         <v>25</v>
       </c>
@@ -33715,7 +33871,7 @@
       </c>
     </row>
     <row r="230" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A230" s="44"/>
+      <c r="A230" s="45"/>
       <c r="B230" s="17">
         <v>26</v>
       </c>
@@ -33845,7 +34001,7 @@
       </c>
     </row>
     <row r="231" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A231" s="44"/>
+      <c r="A231" s="45"/>
       <c r="B231" s="17">
         <v>27</v>
       </c>
@@ -33975,7 +34131,7 @@
       </c>
     </row>
     <row r="232" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A232" s="44"/>
+      <c r="A232" s="45"/>
       <c r="B232" s="17">
         <v>28</v>
       </c>
@@ -34105,7 +34261,7 @@
       </c>
     </row>
     <row r="233" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A233" s="44"/>
+      <c r="A233" s="45"/>
       <c r="B233" s="17">
         <v>29</v>
       </c>
@@ -34235,7 +34391,7 @@
       </c>
     </row>
     <row r="234" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A234" s="44"/>
+      <c r="A234" s="45"/>
       <c r="B234" s="17">
         <v>30</v>
       </c>
@@ -34365,7 +34521,7 @@
       </c>
     </row>
     <row r="235" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A235" s="44"/>
+      <c r="A235" s="45"/>
       <c r="B235" s="17">
         <v>31</v>
       </c>
@@ -34495,7 +34651,7 @@
       </c>
     </row>
     <row r="236" spans="1:373" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A236" s="44"/>
+      <c r="A236" s="45"/>
       <c r="B236" s="21">
         <v>32</v>
       </c>
@@ -34954,7 +35110,7 @@
       <c r="NI236" s="5"/>
     </row>
     <row r="237" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A237" s="44"/>
+      <c r="A237" s="45"/>
       <c r="B237" s="17">
         <v>33</v>
       </c>
@@ -35083,7 +35239,7 @@
       </c>
     </row>
     <row r="238" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A238" s="44"/>
+      <c r="A238" s="45"/>
       <c r="B238" s="17">
         <v>34</v>
       </c>
@@ -35212,7 +35368,7 @@
       </c>
     </row>
     <row r="239" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A239" s="44"/>
+      <c r="A239" s="45"/>
       <c r="B239" s="17">
         <v>35</v>
       </c>
@@ -35341,7 +35497,7 @@
       </c>
     </row>
     <row r="240" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A240" s="44"/>
+      <c r="A240" s="45"/>
       <c r="B240" s="17">
         <v>36</v>
       </c>
@@ -35470,7 +35626,7 @@
       </c>
     </row>
     <row r="241" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A241" s="44"/>
+      <c r="A241" s="45"/>
       <c r="B241" s="17">
         <v>37</v>
       </c>
@@ -35599,7 +35755,7 @@
       </c>
     </row>
     <row r="242" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A242" s="44"/>
+      <c r="A242" s="45"/>
       <c r="B242" s="17">
         <v>38</v>
       </c>
@@ -35728,7 +35884,7 @@
       </c>
     </row>
     <row r="243" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A243" s="44"/>
+      <c r="A243" s="45"/>
       <c r="B243" s="17">
         <v>39</v>
       </c>
@@ -35857,7 +36013,7 @@
       </c>
     </row>
     <row r="244" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A244" s="45"/>
+      <c r="A244" s="46"/>
       <c r="B244" s="27">
         <v>40</v>
       </c>
@@ -35986,7 +36142,7 @@
       </c>
     </row>
     <row r="245" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A245" s="46">
+      <c r="A245" s="43">
         <v>7</v>
       </c>
       <c r="B245" s="17">
@@ -36118,7 +36274,7 @@
       </c>
     </row>
     <row r="246" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A246" s="46"/>
+      <c r="A246" s="43"/>
       <c r="B246" s="17">
         <v>2</v>
       </c>
@@ -36248,7 +36404,7 @@
       </c>
     </row>
     <row r="247" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A247" s="46"/>
+      <c r="A247" s="43"/>
       <c r="B247" s="17">
         <v>3</v>
       </c>
@@ -36378,7 +36534,7 @@
       </c>
     </row>
     <row r="248" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A248" s="46"/>
+      <c r="A248" s="43"/>
       <c r="B248" s="17">
         <v>4</v>
       </c>
@@ -36508,7 +36664,7 @@
       </c>
     </row>
     <row r="249" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A249" s="46"/>
+      <c r="A249" s="43"/>
       <c r="B249" s="17">
         <v>5</v>
       </c>
@@ -36638,7 +36794,7 @@
       </c>
     </row>
     <row r="250" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A250" s="46"/>
+      <c r="A250" s="43"/>
       <c r="B250" s="17">
         <v>6</v>
       </c>
@@ -36768,7 +36924,7 @@
       </c>
     </row>
     <row r="251" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A251" s="46"/>
+      <c r="A251" s="43"/>
       <c r="B251" s="17">
         <v>7</v>
       </c>
@@ -36898,7 +37054,7 @@
       </c>
     </row>
     <row r="252" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A252" s="46"/>
+      <c r="A252" s="43"/>
       <c r="B252" s="17">
         <v>8</v>
       </c>
@@ -37028,7 +37184,7 @@
       </c>
     </row>
     <row r="253" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A253" s="46"/>
+      <c r="A253" s="43"/>
       <c r="B253" s="17">
         <v>9</v>
       </c>
@@ -37158,7 +37314,7 @@
       </c>
     </row>
     <row r="254" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A254" s="46"/>
+      <c r="A254" s="43"/>
       <c r="B254" s="17">
         <v>10</v>
       </c>
@@ -37288,7 +37444,7 @@
       </c>
     </row>
     <row r="255" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A255" s="46"/>
+      <c r="A255" s="43"/>
       <c r="B255" s="17">
         <v>11</v>
       </c>
@@ -37418,7 +37574,7 @@
       </c>
     </row>
     <row r="256" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A256" s="46"/>
+      <c r="A256" s="43"/>
       <c r="B256" s="17">
         <v>12</v>
       </c>
@@ -37548,7 +37704,7 @@
       </c>
     </row>
     <row r="257" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A257" s="46"/>
+      <c r="A257" s="43"/>
       <c r="B257" s="17">
         <v>13</v>
       </c>
@@ -37678,7 +37834,7 @@
       </c>
     </row>
     <row r="258" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A258" s="46"/>
+      <c r="A258" s="43"/>
       <c r="B258" s="17">
         <v>14</v>
       </c>
@@ -37808,7 +37964,7 @@
       </c>
     </row>
     <row r="259" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A259" s="46"/>
+      <c r="A259" s="43"/>
       <c r="B259" s="17">
         <v>15</v>
       </c>
@@ -37938,7 +38094,7 @@
       </c>
     </row>
     <row r="260" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A260" s="46"/>
+      <c r="A260" s="43"/>
       <c r="B260" s="17">
         <v>16</v>
       </c>
@@ -38068,7 +38224,7 @@
       </c>
     </row>
     <row r="261" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A261" s="46"/>
+      <c r="A261" s="43"/>
       <c r="B261" s="17">
         <v>17</v>
       </c>
@@ -38198,7 +38354,7 @@
       </c>
     </row>
     <row r="262" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A262" s="46"/>
+      <c r="A262" s="43"/>
       <c r="B262" s="17">
         <v>18</v>
       </c>
@@ -38328,7 +38484,7 @@
       </c>
     </row>
     <row r="263" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A263" s="46"/>
+      <c r="A263" s="43"/>
       <c r="B263" s="17">
         <v>19</v>
       </c>
@@ -38458,7 +38614,7 @@
       </c>
     </row>
     <row r="264" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A264" s="46"/>
+      <c r="A264" s="43"/>
       <c r="B264" s="17">
         <v>20</v>
       </c>
@@ -38588,7 +38744,7 @@
       </c>
     </row>
     <row r="265" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A265" s="46"/>
+      <c r="A265" s="43"/>
       <c r="B265" s="17">
         <v>21</v>
       </c>
@@ -38718,7 +38874,7 @@
       </c>
     </row>
     <row r="266" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A266" s="46"/>
+      <c r="A266" s="43"/>
       <c r="B266" s="17">
         <v>22</v>
       </c>
@@ -38848,7 +39004,7 @@
       </c>
     </row>
     <row r="267" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A267" s="46"/>
+      <c r="A267" s="43"/>
       <c r="B267" s="17">
         <v>23</v>
       </c>
@@ -38978,7 +39134,7 @@
       </c>
     </row>
     <row r="268" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A268" s="46"/>
+      <c r="A268" s="43"/>
       <c r="B268" s="17">
         <v>24</v>
       </c>
@@ -39108,7 +39264,7 @@
       </c>
     </row>
     <row r="269" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A269" s="46"/>
+      <c r="A269" s="43"/>
       <c r="B269" s="17">
         <v>25</v>
       </c>
@@ -39238,7 +39394,7 @@
       </c>
     </row>
     <row r="270" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A270" s="46"/>
+      <c r="A270" s="43"/>
       <c r="B270" s="17">
         <v>26</v>
       </c>
@@ -39368,7 +39524,7 @@
       </c>
     </row>
     <row r="271" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A271" s="46"/>
+      <c r="A271" s="43"/>
       <c r="B271" s="17">
         <v>27</v>
       </c>
@@ -39498,7 +39654,7 @@
       </c>
     </row>
     <row r="272" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A272" s="46"/>
+      <c r="A272" s="43"/>
       <c r="B272" s="17">
         <v>28</v>
       </c>
@@ -39628,7 +39784,7 @@
       </c>
     </row>
     <row r="273" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A273" s="46"/>
+      <c r="A273" s="43"/>
       <c r="B273" s="17">
         <v>29</v>
       </c>
@@ -39758,7 +39914,7 @@
       </c>
     </row>
     <row r="274" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A274" s="46"/>
+      <c r="A274" s="43"/>
       <c r="B274" s="17">
         <v>30</v>
       </c>
@@ -39888,7 +40044,7 @@
       </c>
     </row>
     <row r="275" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A275" s="46"/>
+      <c r="A275" s="43"/>
       <c r="B275" s="17">
         <v>31</v>
       </c>
@@ -40018,7 +40174,7 @@
       </c>
     </row>
     <row r="276" spans="1:373" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A276" s="46"/>
+      <c r="A276" s="43"/>
       <c r="B276" s="21">
         <v>32</v>
       </c>
@@ -40477,7 +40633,7 @@
       <c r="NI276" s="5"/>
     </row>
     <row r="277" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A277" s="46"/>
+      <c r="A277" s="43"/>
       <c r="B277" s="17">
         <v>33</v>
       </c>
@@ -40606,7 +40762,7 @@
       </c>
     </row>
     <row r="278" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A278" s="46"/>
+      <c r="A278" s="43"/>
       <c r="B278" s="17">
         <v>34</v>
       </c>
@@ -40735,7 +40891,7 @@
       </c>
     </row>
     <row r="279" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A279" s="46"/>
+      <c r="A279" s="43"/>
       <c r="B279" s="17">
         <v>35</v>
       </c>
@@ -40864,7 +41020,7 @@
       </c>
     </row>
     <row r="280" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A280" s="46"/>
+      <c r="A280" s="43"/>
       <c r="B280" s="17">
         <v>36</v>
       </c>
@@ -40993,7 +41149,7 @@
       </c>
     </row>
     <row r="281" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A281" s="46"/>
+      <c r="A281" s="43"/>
       <c r="B281" s="17">
         <v>37</v>
       </c>
@@ -41122,7 +41278,7 @@
       </c>
     </row>
     <row r="282" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A282" s="46"/>
+      <c r="A282" s="43"/>
       <c r="B282" s="17">
         <v>38</v>
       </c>
@@ -41251,7 +41407,7 @@
       </c>
     </row>
     <row r="283" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A283" s="46"/>
+      <c r="A283" s="43"/>
       <c r="B283" s="17">
         <v>39</v>
       </c>
@@ -41380,7 +41536,7 @@
       </c>
     </row>
     <row r="284" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A284" s="46"/>
+      <c r="A284" s="43"/>
       <c r="B284" s="17">
         <v>40</v>
       </c>
@@ -41509,7 +41665,7 @@
       </c>
     </row>
     <row r="285" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A285" s="43">
+      <c r="A285" s="44">
         <v>8</v>
       </c>
       <c r="B285" s="21">
@@ -41641,7 +41797,7 @@
       </c>
     </row>
     <row r="286" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A286" s="44"/>
+      <c r="A286" s="45"/>
       <c r="B286" s="17">
         <v>2</v>
       </c>
@@ -41771,7 +41927,7 @@
       </c>
     </row>
     <row r="287" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A287" s="44"/>
+      <c r="A287" s="45"/>
       <c r="B287" s="17">
         <v>3</v>
       </c>
@@ -41901,7 +42057,7 @@
       </c>
     </row>
     <row r="288" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A288" s="44"/>
+      <c r="A288" s="45"/>
       <c r="B288" s="17">
         <v>4</v>
       </c>
@@ -42031,7 +42187,7 @@
       </c>
     </row>
     <row r="289" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A289" s="44"/>
+      <c r="A289" s="45"/>
       <c r="B289" s="17">
         <v>5</v>
       </c>
@@ -42161,7 +42317,7 @@
       </c>
     </row>
     <row r="290" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A290" s="44"/>
+      <c r="A290" s="45"/>
       <c r="B290" s="17">
         <v>6</v>
       </c>
@@ -42291,7 +42447,7 @@
       </c>
     </row>
     <row r="291" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A291" s="44"/>
+      <c r="A291" s="45"/>
       <c r="B291" s="17">
         <v>7</v>
       </c>
@@ -42421,7 +42577,7 @@
       </c>
     </row>
     <row r="292" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A292" s="44"/>
+      <c r="A292" s="45"/>
       <c r="B292" s="17">
         <v>8</v>
       </c>
@@ -42551,7 +42707,7 @@
       </c>
     </row>
     <row r="293" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A293" s="44"/>
+      <c r="A293" s="45"/>
       <c r="B293" s="17">
         <v>9</v>
       </c>
@@ -42681,7 +42837,7 @@
       </c>
     </row>
     <row r="294" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A294" s="44"/>
+      <c r="A294" s="45"/>
       <c r="B294" s="17">
         <v>10</v>
       </c>
@@ -42811,7 +42967,7 @@
       </c>
     </row>
     <row r="295" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A295" s="44"/>
+      <c r="A295" s="45"/>
       <c r="B295" s="17">
         <v>11</v>
       </c>
@@ -42941,7 +43097,7 @@
       </c>
     </row>
     <row r="296" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A296" s="44"/>
+      <c r="A296" s="45"/>
       <c r="B296" s="17">
         <v>12</v>
       </c>
@@ -43071,7 +43227,7 @@
       </c>
     </row>
     <row r="297" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A297" s="44"/>
+      <c r="A297" s="45"/>
       <c r="B297" s="17">
         <v>13</v>
       </c>
@@ -43201,7 +43357,7 @@
       </c>
     </row>
     <row r="298" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A298" s="44"/>
+      <c r="A298" s="45"/>
       <c r="B298" s="17">
         <v>14</v>
       </c>
@@ -43331,7 +43487,7 @@
       </c>
     </row>
     <row r="299" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A299" s="44"/>
+      <c r="A299" s="45"/>
       <c r="B299" s="17">
         <v>15</v>
       </c>
@@ -43461,7 +43617,7 @@
       </c>
     </row>
     <row r="300" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A300" s="44"/>
+      <c r="A300" s="45"/>
       <c r="B300" s="17">
         <v>16</v>
       </c>
@@ -43591,7 +43747,7 @@
       </c>
     </row>
     <row r="301" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A301" s="44"/>
+      <c r="A301" s="45"/>
       <c r="B301" s="17">
         <v>17</v>
       </c>
@@ -43721,7 +43877,7 @@
       </c>
     </row>
     <row r="302" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A302" s="44"/>
+      <c r="A302" s="45"/>
       <c r="B302" s="17">
         <v>18</v>
       </c>
@@ -43851,7 +44007,7 @@
       </c>
     </row>
     <row r="303" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A303" s="44"/>
+      <c r="A303" s="45"/>
       <c r="B303" s="17">
         <v>19</v>
       </c>
@@ -43981,7 +44137,7 @@
       </c>
     </row>
     <row r="304" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A304" s="44"/>
+      <c r="A304" s="45"/>
       <c r="B304" s="17">
         <v>20</v>
       </c>
@@ -44111,7 +44267,7 @@
       </c>
     </row>
     <row r="305" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A305" s="44"/>
+      <c r="A305" s="45"/>
       <c r="B305" s="17">
         <v>21</v>
       </c>
@@ -44241,7 +44397,7 @@
       </c>
     </row>
     <row r="306" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A306" s="44"/>
+      <c r="A306" s="45"/>
       <c r="B306" s="17">
         <v>22</v>
       </c>
@@ -44371,7 +44527,7 @@
       </c>
     </row>
     <row r="307" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A307" s="44"/>
+      <c r="A307" s="45"/>
       <c r="B307" s="17">
         <v>23</v>
       </c>
@@ -44501,7 +44657,7 @@
       </c>
     </row>
     <row r="308" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A308" s="44"/>
+      <c r="A308" s="45"/>
       <c r="B308" s="17">
         <v>24</v>
       </c>
@@ -44631,7 +44787,7 @@
       </c>
     </row>
     <row r="309" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A309" s="44"/>
+      <c r="A309" s="45"/>
       <c r="B309" s="17">
         <v>25</v>
       </c>
@@ -44761,7 +44917,7 @@
       </c>
     </row>
     <row r="310" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A310" s="44"/>
+      <c r="A310" s="45"/>
       <c r="B310" s="17">
         <v>26</v>
       </c>
@@ -44891,7 +45047,7 @@
       </c>
     </row>
     <row r="311" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A311" s="44"/>
+      <c r="A311" s="45"/>
       <c r="B311" s="17">
         <v>27</v>
       </c>
@@ -45021,7 +45177,7 @@
       </c>
     </row>
     <row r="312" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A312" s="44"/>
+      <c r="A312" s="45"/>
       <c r="B312" s="17">
         <v>28</v>
       </c>
@@ -45151,7 +45307,7 @@
       </c>
     </row>
     <row r="313" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A313" s="44"/>
+      <c r="A313" s="45"/>
       <c r="B313" s="17">
         <v>29</v>
       </c>
@@ -45281,7 +45437,7 @@
       </c>
     </row>
     <row r="314" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A314" s="44"/>
+      <c r="A314" s="45"/>
       <c r="B314" s="17">
         <v>30</v>
       </c>
@@ -45411,7 +45567,7 @@
       </c>
     </row>
     <row r="315" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A315" s="44"/>
+      <c r="A315" s="45"/>
       <c r="B315" s="17">
         <v>31</v>
       </c>
@@ -45541,7 +45697,7 @@
       </c>
     </row>
     <row r="316" spans="1:373" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A316" s="44"/>
+      <c r="A316" s="45"/>
       <c r="B316" s="21">
         <v>32</v>
       </c>
@@ -46000,7 +46156,7 @@
       <c r="NI316" s="5"/>
     </row>
     <row r="317" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A317" s="44"/>
+      <c r="A317" s="45"/>
       <c r="B317" s="17">
         <v>33</v>
       </c>
@@ -46129,7 +46285,7 @@
       </c>
     </row>
     <row r="318" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A318" s="44"/>
+      <c r="A318" s="45"/>
       <c r="B318" s="17">
         <v>34</v>
       </c>
@@ -46258,7 +46414,7 @@
       </c>
     </row>
     <row r="319" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A319" s="44"/>
+      <c r="A319" s="45"/>
       <c r="B319" s="17">
         <v>35</v>
       </c>
@@ -46387,7 +46543,7 @@
       </c>
     </row>
     <row r="320" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A320" s="44"/>
+      <c r="A320" s="45"/>
       <c r="B320" s="17">
         <v>36</v>
       </c>
@@ -46516,7 +46672,7 @@
       </c>
     </row>
     <row r="321" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A321" s="44"/>
+      <c r="A321" s="45"/>
       <c r="B321" s="17">
         <v>37</v>
       </c>
@@ -46645,7 +46801,7 @@
       </c>
     </row>
     <row r="322" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A322" s="44"/>
+      <c r="A322" s="45"/>
       <c r="B322" s="17">
         <v>38</v>
       </c>
@@ -46774,7 +46930,7 @@
       </c>
     </row>
     <row r="323" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A323" s="44"/>
+      <c r="A323" s="45"/>
       <c r="B323" s="17">
         <v>39</v>
       </c>
@@ -46903,7 +47059,7 @@
       </c>
     </row>
     <row r="324" spans="1:43" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A324" s="45"/>
+      <c r="A324" s="46"/>
       <c r="B324" s="27">
         <v>40</v>
       </c>
@@ -47032,7 +47188,7 @@
       </c>
     </row>
     <row r="325" spans="1:43" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A325" s="46">
+      <c r="A325" s="43">
         <v>9</v>
       </c>
       <c r="B325" s="17">
@@ -47164,7 +47320,7 @@
       </c>
     </row>
     <row r="326" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A326" s="46"/>
+      <c r="A326" s="43"/>
       <c r="B326" s="17">
         <v>2</v>
       </c>
@@ -47294,7 +47450,7 @@
       </c>
     </row>
     <row r="327" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A327" s="46"/>
+      <c r="A327" s="43"/>
       <c r="B327" s="17">
         <v>3</v>
       </c>
@@ -47424,7 +47580,7 @@
       </c>
     </row>
     <row r="328" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A328" s="46"/>
+      <c r="A328" s="43"/>
       <c r="B328" s="17">
         <v>4</v>
       </c>
@@ -47554,7 +47710,7 @@
       </c>
     </row>
     <row r="329" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A329" s="46"/>
+      <c r="A329" s="43"/>
       <c r="B329" s="17">
         <v>5</v>
       </c>
@@ -47684,7 +47840,7 @@
       </c>
     </row>
     <row r="330" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A330" s="46"/>
+      <c r="A330" s="43"/>
       <c r="B330" s="17">
         <v>6</v>
       </c>
@@ -47814,7 +47970,7 @@
       </c>
     </row>
     <row r="331" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A331" s="46"/>
+      <c r="A331" s="43"/>
       <c r="B331" s="17">
         <v>7</v>
       </c>
@@ -47944,7 +48100,7 @@
       </c>
     </row>
     <row r="332" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A332" s="46"/>
+      <c r="A332" s="43"/>
       <c r="B332" s="17">
         <v>8</v>
       </c>
@@ -48074,7 +48230,7 @@
       </c>
     </row>
     <row r="333" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A333" s="46"/>
+      <c r="A333" s="43"/>
       <c r="B333" s="17">
         <v>9</v>
       </c>
@@ -48204,7 +48360,7 @@
       </c>
     </row>
     <row r="334" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A334" s="46"/>
+      <c r="A334" s="43"/>
       <c r="B334" s="17">
         <v>10</v>
       </c>
@@ -48334,7 +48490,7 @@
       </c>
     </row>
     <row r="335" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A335" s="46"/>
+      <c r="A335" s="43"/>
       <c r="B335" s="17">
         <v>11</v>
       </c>
@@ -48464,7 +48620,7 @@
       </c>
     </row>
     <row r="336" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A336" s="46"/>
+      <c r="A336" s="43"/>
       <c r="B336" s="17">
         <v>12</v>
       </c>
@@ -48594,7 +48750,7 @@
       </c>
     </row>
     <row r="337" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A337" s="46"/>
+      <c r="A337" s="43"/>
       <c r="B337" s="17">
         <v>13</v>
       </c>
@@ -48724,7 +48880,7 @@
       </c>
     </row>
     <row r="338" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A338" s="46"/>
+      <c r="A338" s="43"/>
       <c r="B338" s="17">
         <v>14</v>
       </c>
@@ -48854,7 +49010,7 @@
       </c>
     </row>
     <row r="339" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A339" s="46"/>
+      <c r="A339" s="43"/>
       <c r="B339" s="17">
         <v>15</v>
       </c>
@@ -48984,7 +49140,7 @@
       </c>
     </row>
     <row r="340" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A340" s="46"/>
+      <c r="A340" s="43"/>
       <c r="B340" s="17">
         <v>16</v>
       </c>
@@ -49114,7 +49270,7 @@
       </c>
     </row>
     <row r="341" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A341" s="46"/>
+      <c r="A341" s="43"/>
       <c r="B341" s="17">
         <v>17</v>
       </c>
@@ -49244,7 +49400,7 @@
       </c>
     </row>
     <row r="342" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A342" s="46"/>
+      <c r="A342" s="43"/>
       <c r="B342" s="17">
         <v>18</v>
       </c>
@@ -49374,7 +49530,7 @@
       </c>
     </row>
     <row r="343" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A343" s="46"/>
+      <c r="A343" s="43"/>
       <c r="B343" s="17">
         <v>19</v>
       </c>
@@ -49504,7 +49660,7 @@
       </c>
     </row>
     <row r="344" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A344" s="46"/>
+      <c r="A344" s="43"/>
       <c r="B344" s="17">
         <v>20</v>
       </c>
@@ -49634,7 +49790,7 @@
       </c>
     </row>
     <row r="345" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A345" s="46"/>
+      <c r="A345" s="43"/>
       <c r="B345" s="17">
         <v>21</v>
       </c>
@@ -49764,7 +49920,7 @@
       </c>
     </row>
     <row r="346" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A346" s="46"/>
+      <c r="A346" s="43"/>
       <c r="B346" s="17">
         <v>22</v>
       </c>
@@ -49894,7 +50050,7 @@
       </c>
     </row>
     <row r="347" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A347" s="46"/>
+      <c r="A347" s="43"/>
       <c r="B347" s="17">
         <v>23</v>
       </c>
@@ -50024,7 +50180,7 @@
       </c>
     </row>
     <row r="348" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A348" s="46"/>
+      <c r="A348" s="43"/>
       <c r="B348" s="17">
         <v>24</v>
       </c>
@@ -50154,7 +50310,7 @@
       </c>
     </row>
     <row r="349" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A349" s="46"/>
+      <c r="A349" s="43"/>
       <c r="B349" s="17">
         <v>25</v>
       </c>
@@ -50284,7 +50440,7 @@
       </c>
     </row>
     <row r="350" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A350" s="46"/>
+      <c r="A350" s="43"/>
       <c r="B350" s="17">
         <v>26</v>
       </c>
@@ -50414,7 +50570,7 @@
       </c>
     </row>
     <row r="351" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A351" s="46"/>
+      <c r="A351" s="43"/>
       <c r="B351" s="17">
         <v>27</v>
       </c>
@@ -50544,7 +50700,7 @@
       </c>
     </row>
     <row r="352" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A352" s="46"/>
+      <c r="A352" s="43"/>
       <c r="B352" s="17">
         <v>28</v>
       </c>
@@ -50674,7 +50830,7 @@
       </c>
     </row>
     <row r="353" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A353" s="46"/>
+      <c r="A353" s="43"/>
       <c r="B353" s="17">
         <v>29</v>
       </c>
@@ -50804,7 +50960,7 @@
       </c>
     </row>
     <row r="354" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A354" s="46"/>
+      <c r="A354" s="43"/>
       <c r="B354" s="17">
         <v>30</v>
       </c>
@@ -50934,7 +51090,7 @@
       </c>
     </row>
     <row r="355" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A355" s="46"/>
+      <c r="A355" s="43"/>
       <c r="B355" s="17">
         <v>31</v>
       </c>
@@ -51064,7 +51220,7 @@
       </c>
     </row>
     <row r="356" spans="1:373" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A356" s="46"/>
+      <c r="A356" s="43"/>
       <c r="B356" s="21">
         <v>32</v>
       </c>
@@ -51523,7 +51679,7 @@
       <c r="NI356" s="5"/>
     </row>
     <row r="357" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A357" s="46"/>
+      <c r="A357" s="43"/>
       <c r="B357" s="17">
         <v>33</v>
       </c>
@@ -51652,7 +51808,7 @@
       </c>
     </row>
     <row r="358" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A358" s="46"/>
+      <c r="A358" s="43"/>
       <c r="B358" s="17">
         <v>34</v>
       </c>
@@ -51781,7 +51937,7 @@
       </c>
     </row>
     <row r="359" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A359" s="46"/>
+      <c r="A359" s="43"/>
       <c r="B359" s="17">
         <v>35</v>
       </c>
@@ -51910,7 +52066,7 @@
       </c>
     </row>
     <row r="360" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A360" s="46"/>
+      <c r="A360" s="43"/>
       <c r="B360" s="17">
         <v>36</v>
       </c>
@@ -52039,7 +52195,7 @@
       </c>
     </row>
     <row r="361" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A361" s="46"/>
+      <c r="A361" s="43"/>
       <c r="B361" s="17">
         <v>37</v>
       </c>
@@ -52168,7 +52324,7 @@
       </c>
     </row>
     <row r="362" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A362" s="46"/>
+      <c r="A362" s="43"/>
       <c r="B362" s="17">
         <v>38</v>
       </c>
@@ -52297,7 +52453,7 @@
       </c>
     </row>
     <row r="363" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A363" s="46"/>
+      <c r="A363" s="43"/>
       <c r="B363" s="17">
         <v>39</v>
       </c>
@@ -52426,7 +52582,7 @@
       </c>
     </row>
     <row r="364" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A364" s="46"/>
+      <c r="A364" s="43"/>
       <c r="B364" s="17">
         <v>40</v>
       </c>
@@ -52555,7 +52711,7 @@
       </c>
     </row>
     <row r="365" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A365" s="43">
+      <c r="A365" s="44">
         <v>10</v>
       </c>
       <c r="B365" s="21">
@@ -52687,7 +52843,7 @@
       </c>
     </row>
     <row r="366" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A366" s="44"/>
+      <c r="A366" s="45"/>
       <c r="B366" s="17">
         <v>2</v>
       </c>
@@ -52817,7 +52973,7 @@
       </c>
     </row>
     <row r="367" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A367" s="44"/>
+      <c r="A367" s="45"/>
       <c r="B367" s="17">
         <v>3</v>
       </c>
@@ -52947,7 +53103,7 @@
       </c>
     </row>
     <row r="368" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A368" s="44"/>
+      <c r="A368" s="45"/>
       <c r="B368" s="17">
         <v>4</v>
       </c>
@@ -53077,7 +53233,7 @@
       </c>
     </row>
     <row r="369" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A369" s="44"/>
+      <c r="A369" s="45"/>
       <c r="B369" s="17">
         <v>5</v>
       </c>
@@ -53207,7 +53363,7 @@
       </c>
     </row>
     <row r="370" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A370" s="44"/>
+      <c r="A370" s="45"/>
       <c r="B370" s="17">
         <v>6</v>
       </c>
@@ -53337,7 +53493,7 @@
       </c>
     </row>
     <row r="371" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A371" s="44"/>
+      <c r="A371" s="45"/>
       <c r="B371" s="17">
         <v>7</v>
       </c>
@@ -53467,7 +53623,7 @@
       </c>
     </row>
     <row r="372" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A372" s="44"/>
+      <c r="A372" s="45"/>
       <c r="B372" s="17">
         <v>8</v>
       </c>
@@ -53597,7 +53753,7 @@
       </c>
     </row>
     <row r="373" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A373" s="44"/>
+      <c r="A373" s="45"/>
       <c r="B373" s="17">
         <v>9</v>
       </c>
@@ -53727,7 +53883,7 @@
       </c>
     </row>
     <row r="374" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A374" s="44"/>
+      <c r="A374" s="45"/>
       <c r="B374" s="17">
         <v>10</v>
       </c>
@@ -53857,7 +54013,7 @@
       </c>
     </row>
     <row r="375" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A375" s="44"/>
+      <c r="A375" s="45"/>
       <c r="B375" s="17">
         <v>11</v>
       </c>
@@ -53987,7 +54143,7 @@
       </c>
     </row>
     <row r="376" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A376" s="44"/>
+      <c r="A376" s="45"/>
       <c r="B376" s="17">
         <v>12</v>
       </c>
@@ -54117,7 +54273,7 @@
       </c>
     </row>
     <row r="377" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A377" s="44"/>
+      <c r="A377" s="45"/>
       <c r="B377" s="17">
         <v>13</v>
       </c>
@@ -54247,7 +54403,7 @@
       </c>
     </row>
     <row r="378" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A378" s="44"/>
+      <c r="A378" s="45"/>
       <c r="B378" s="17">
         <v>14</v>
       </c>
@@ -54377,7 +54533,7 @@
       </c>
     </row>
     <row r="379" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A379" s="44"/>
+      <c r="A379" s="45"/>
       <c r="B379" s="17">
         <v>15</v>
       </c>
@@ -54507,7 +54663,7 @@
       </c>
     </row>
     <row r="380" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A380" s="44"/>
+      <c r="A380" s="45"/>
       <c r="B380" s="17">
         <v>16</v>
       </c>
@@ -54637,7 +54793,7 @@
       </c>
     </row>
     <row r="381" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A381" s="44"/>
+      <c r="A381" s="45"/>
       <c r="B381" s="17">
         <v>17</v>
       </c>
@@ -54767,7 +54923,7 @@
       </c>
     </row>
     <row r="382" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A382" s="44"/>
+      <c r="A382" s="45"/>
       <c r="B382" s="17">
         <v>18</v>
       </c>
@@ -54897,7 +55053,7 @@
       </c>
     </row>
     <row r="383" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A383" s="44"/>
+      <c r="A383" s="45"/>
       <c r="B383" s="17">
         <v>19</v>
       </c>
@@ -55027,7 +55183,7 @@
       </c>
     </row>
     <row r="384" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A384" s="44"/>
+      <c r="A384" s="45"/>
       <c r="B384" s="17">
         <v>20</v>
       </c>
@@ -55157,7 +55313,7 @@
       </c>
     </row>
     <row r="385" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A385" s="44"/>
+      <c r="A385" s="45"/>
       <c r="B385" s="17">
         <v>21</v>
       </c>
@@ -55287,7 +55443,7 @@
       </c>
     </row>
     <row r="386" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A386" s="44"/>
+      <c r="A386" s="45"/>
       <c r="B386" s="17">
         <v>22</v>
       </c>
@@ -55417,7 +55573,7 @@
       </c>
     </row>
     <row r="387" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A387" s="44"/>
+      <c r="A387" s="45"/>
       <c r="B387" s="17">
         <v>23</v>
       </c>
@@ -55547,7 +55703,7 @@
       </c>
     </row>
     <row r="388" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A388" s="44"/>
+      <c r="A388" s="45"/>
       <c r="B388" s="17">
         <v>24</v>
       </c>
@@ -55677,7 +55833,7 @@
       </c>
     </row>
     <row r="389" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A389" s="44"/>
+      <c r="A389" s="45"/>
       <c r="B389" s="17">
         <v>25</v>
       </c>
@@ -55807,7 +55963,7 @@
       </c>
     </row>
     <row r="390" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A390" s="44"/>
+      <c r="A390" s="45"/>
       <c r="B390" s="17">
         <v>26</v>
       </c>
@@ -55937,7 +56093,7 @@
       </c>
     </row>
     <row r="391" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A391" s="44"/>
+      <c r="A391" s="45"/>
       <c r="B391" s="17">
         <v>27</v>
       </c>
@@ -56067,7 +56223,7 @@
       </c>
     </row>
     <row r="392" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A392" s="44"/>
+      <c r="A392" s="45"/>
       <c r="B392" s="17">
         <v>28</v>
       </c>
@@ -56197,7 +56353,7 @@
       </c>
     </row>
     <row r="393" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A393" s="44"/>
+      <c r="A393" s="45"/>
       <c r="B393" s="17">
         <v>29</v>
       </c>
@@ -56327,7 +56483,7 @@
       </c>
     </row>
     <row r="394" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A394" s="44"/>
+      <c r="A394" s="45"/>
       <c r="B394" s="17">
         <v>30</v>
       </c>
@@ -56457,7 +56613,7 @@
       </c>
     </row>
     <row r="395" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A395" s="44"/>
+      <c r="A395" s="45"/>
       <c r="B395" s="17">
         <v>31</v>
       </c>
@@ -56587,7 +56743,7 @@
       </c>
     </row>
     <row r="396" spans="1:373" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A396" s="44"/>
+      <c r="A396" s="45"/>
       <c r="B396" s="21">
         <v>32</v>
       </c>
@@ -57046,7 +57202,7 @@
       <c r="NI396" s="5"/>
     </row>
     <row r="397" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A397" s="44"/>
+      <c r="A397" s="45"/>
       <c r="B397" s="17">
         <v>33</v>
       </c>
@@ -57175,7 +57331,7 @@
       </c>
     </row>
     <row r="398" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A398" s="44"/>
+      <c r="A398" s="45"/>
       <c r="B398" s="17">
         <v>34</v>
       </c>
@@ -57304,7 +57460,7 @@
       </c>
     </row>
     <row r="399" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A399" s="44"/>
+      <c r="A399" s="45"/>
       <c r="B399" s="17">
         <v>35</v>
       </c>
@@ -57433,7 +57589,7 @@
       </c>
     </row>
     <row r="400" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A400" s="44"/>
+      <c r="A400" s="45"/>
       <c r="B400" s="17">
         <v>36</v>
       </c>
@@ -57562,7 +57718,7 @@
       </c>
     </row>
     <row r="401" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A401" s="44"/>
+      <c r="A401" s="45"/>
       <c r="B401" s="17">
         <v>37</v>
       </c>
@@ -57691,7 +57847,7 @@
       </c>
     </row>
     <row r="402" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A402" s="44"/>
+      <c r="A402" s="45"/>
       <c r="B402" s="17">
         <v>38</v>
       </c>
@@ -57820,7 +57976,7 @@
       </c>
     </row>
     <row r="403" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A403" s="44"/>
+      <c r="A403" s="45"/>
       <c r="B403" s="17">
         <v>39</v>
       </c>
@@ -57949,7 +58105,7 @@
       </c>
     </row>
     <row r="404" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A404" s="45"/>
+      <c r="A404" s="46"/>
       <c r="B404" s="27">
         <v>40</v>
       </c>
@@ -58078,7 +58234,7 @@
       </c>
     </row>
     <row r="405" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A405" s="46">
+      <c r="A405" s="43">
         <v>11</v>
       </c>
       <c r="B405" s="17">
@@ -58210,7 +58366,7 @@
       </c>
     </row>
     <row r="406" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A406" s="46"/>
+      <c r="A406" s="43"/>
       <c r="B406" s="17">
         <v>2</v>
       </c>
@@ -58340,7 +58496,7 @@
       </c>
     </row>
     <row r="407" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A407" s="46"/>
+      <c r="A407" s="43"/>
       <c r="B407" s="17">
         <v>3</v>
       </c>
@@ -58470,7 +58626,7 @@
       </c>
     </row>
     <row r="408" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A408" s="46"/>
+      <c r="A408" s="43"/>
       <c r="B408" s="17">
         <v>4</v>
       </c>
@@ -58600,7 +58756,7 @@
       </c>
     </row>
     <row r="409" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A409" s="46"/>
+      <c r="A409" s="43"/>
       <c r="B409" s="17">
         <v>5</v>
       </c>
@@ -58730,7 +58886,7 @@
       </c>
     </row>
     <row r="410" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A410" s="46"/>
+      <c r="A410" s="43"/>
       <c r="B410" s="17">
         <v>6</v>
       </c>
@@ -58860,7 +59016,7 @@
       </c>
     </row>
     <row r="411" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A411" s="46"/>
+      <c r="A411" s="43"/>
       <c r="B411" s="17">
         <v>7</v>
       </c>
@@ -58990,7 +59146,7 @@
       </c>
     </row>
     <row r="412" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A412" s="46"/>
+      <c r="A412" s="43"/>
       <c r="B412" s="17">
         <v>8</v>
       </c>
@@ -59120,7 +59276,7 @@
       </c>
     </row>
     <row r="413" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A413" s="46"/>
+      <c r="A413" s="43"/>
       <c r="B413" s="17">
         <v>9</v>
       </c>
@@ -59250,7 +59406,7 @@
       </c>
     </row>
     <row r="414" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A414" s="46"/>
+      <c r="A414" s="43"/>
       <c r="B414" s="17">
         <v>10</v>
       </c>
@@ -59380,7 +59536,7 @@
       </c>
     </row>
     <row r="415" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A415" s="46"/>
+      <c r="A415" s="43"/>
       <c r="B415" s="17">
         <v>11</v>
       </c>
@@ -59510,7 +59666,7 @@
       </c>
     </row>
     <row r="416" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A416" s="46"/>
+      <c r="A416" s="43"/>
       <c r="B416" s="17">
         <v>12</v>
       </c>
@@ -59640,7 +59796,7 @@
       </c>
     </row>
     <row r="417" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A417" s="46"/>
+      <c r="A417" s="43"/>
       <c r="B417" s="17">
         <v>13</v>
       </c>
@@ -59770,7 +59926,7 @@
       </c>
     </row>
     <row r="418" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A418" s="46"/>
+      <c r="A418" s="43"/>
       <c r="B418" s="17">
         <v>14</v>
       </c>
@@ -59900,7 +60056,7 @@
       </c>
     </row>
     <row r="419" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A419" s="46"/>
+      <c r="A419" s="43"/>
       <c r="B419" s="17">
         <v>15</v>
       </c>
@@ -60030,7 +60186,7 @@
       </c>
     </row>
     <row r="420" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A420" s="46"/>
+      <c r="A420" s="43"/>
       <c r="B420" s="17">
         <v>16</v>
       </c>
@@ -60160,7 +60316,7 @@
       </c>
     </row>
     <row r="421" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A421" s="46"/>
+      <c r="A421" s="43"/>
       <c r="B421" s="17">
         <v>17</v>
       </c>
@@ -60290,7 +60446,7 @@
       </c>
     </row>
     <row r="422" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A422" s="46"/>
+      <c r="A422" s="43"/>
       <c r="B422" s="17">
         <v>18</v>
       </c>
@@ -60420,7 +60576,7 @@
       </c>
     </row>
     <row r="423" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A423" s="46"/>
+      <c r="A423" s="43"/>
       <c r="B423" s="17">
         <v>19</v>
       </c>
@@ -60550,7 +60706,7 @@
       </c>
     </row>
     <row r="424" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A424" s="46"/>
+      <c r="A424" s="43"/>
       <c r="B424" s="17">
         <v>20</v>
       </c>
@@ -60680,7 +60836,7 @@
       </c>
     </row>
     <row r="425" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A425" s="46"/>
+      <c r="A425" s="43"/>
       <c r="B425" s="17">
         <v>21</v>
       </c>
@@ -60810,7 +60966,7 @@
       </c>
     </row>
     <row r="426" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A426" s="46"/>
+      <c r="A426" s="43"/>
       <c r="B426" s="17">
         <v>22</v>
       </c>
@@ -60940,7 +61096,7 @@
       </c>
     </row>
     <row r="427" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A427" s="46"/>
+      <c r="A427" s="43"/>
       <c r="B427" s="17">
         <v>23</v>
       </c>
@@ -61070,7 +61226,7 @@
       </c>
     </row>
     <row r="428" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A428" s="46"/>
+      <c r="A428" s="43"/>
       <c r="B428" s="17">
         <v>24</v>
       </c>
@@ -61200,7 +61356,7 @@
       </c>
     </row>
     <row r="429" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A429" s="46"/>
+      <c r="A429" s="43"/>
       <c r="B429" s="17">
         <v>25</v>
       </c>
@@ -61330,7 +61486,7 @@
       </c>
     </row>
     <row r="430" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A430" s="46"/>
+      <c r="A430" s="43"/>
       <c r="B430" s="17">
         <v>26</v>
       </c>
@@ -61460,7 +61616,7 @@
       </c>
     </row>
     <row r="431" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A431" s="46"/>
+      <c r="A431" s="43"/>
       <c r="B431" s="17">
         <v>27</v>
       </c>
@@ -61590,7 +61746,7 @@
       </c>
     </row>
     <row r="432" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A432" s="46"/>
+      <c r="A432" s="43"/>
       <c r="B432" s="17">
         <v>28</v>
       </c>
@@ -61720,7 +61876,7 @@
       </c>
     </row>
     <row r="433" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A433" s="46"/>
+      <c r="A433" s="43"/>
       <c r="B433" s="17">
         <v>29</v>
       </c>
@@ -61850,7 +62006,7 @@
       </c>
     </row>
     <row r="434" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A434" s="46"/>
+      <c r="A434" s="43"/>
       <c r="B434" s="17">
         <v>30</v>
       </c>
@@ -61980,7 +62136,7 @@
       </c>
     </row>
     <row r="435" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A435" s="46"/>
+      <c r="A435" s="43"/>
       <c r="B435" s="17">
         <v>31</v>
       </c>
@@ -62110,7 +62266,7 @@
       </c>
     </row>
     <row r="436" spans="1:373" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A436" s="46"/>
+      <c r="A436" s="43"/>
       <c r="B436" s="21">
         <v>32</v>
       </c>
@@ -62569,7 +62725,7 @@
       <c r="NI436" s="5"/>
     </row>
     <row r="437" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A437" s="46"/>
+      <c r="A437" s="43"/>
       <c r="B437" s="17">
         <v>33</v>
       </c>
@@ -62698,7 +62854,7 @@
       </c>
     </row>
     <row r="438" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A438" s="46"/>
+      <c r="A438" s="43"/>
       <c r="B438" s="17">
         <v>34</v>
       </c>
@@ -62827,7 +62983,7 @@
       </c>
     </row>
     <row r="439" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A439" s="46"/>
+      <c r="A439" s="43"/>
       <c r="B439" s="17">
         <v>35</v>
       </c>
@@ -62956,7 +63112,7 @@
       </c>
     </row>
     <row r="440" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A440" s="46"/>
+      <c r="A440" s="43"/>
       <c r="B440" s="17">
         <v>36</v>
       </c>
@@ -63085,7 +63241,7 @@
       </c>
     </row>
     <row r="441" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A441" s="46"/>
+      <c r="A441" s="43"/>
       <c r="B441" s="17">
         <v>37</v>
       </c>
@@ -63214,7 +63370,7 @@
       </c>
     </row>
     <row r="442" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A442" s="46"/>
+      <c r="A442" s="43"/>
       <c r="B442" s="17">
         <v>38</v>
       </c>
@@ -63343,7 +63499,7 @@
       </c>
     </row>
     <row r="443" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A443" s="46"/>
+      <c r="A443" s="43"/>
       <c r="B443" s="17">
         <v>39</v>
       </c>
@@ -63472,7 +63628,7 @@
       </c>
     </row>
     <row r="444" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A444" s="46"/>
+      <c r="A444" s="43"/>
       <c r="B444" s="17">
         <v>40</v>
       </c>
@@ -63601,7 +63757,7 @@
       </c>
     </row>
     <row r="445" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A445" s="43">
+      <c r="A445" s="44">
         <v>12</v>
       </c>
       <c r="B445" s="21">
@@ -63733,7 +63889,7 @@
       </c>
     </row>
     <row r="446" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A446" s="44"/>
+      <c r="A446" s="45"/>
       <c r="B446" s="17">
         <v>2</v>
       </c>
@@ -63863,7 +64019,7 @@
       </c>
     </row>
     <row r="447" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A447" s="44"/>
+      <c r="A447" s="45"/>
       <c r="B447" s="17">
         <v>3</v>
       </c>
@@ -63993,7 +64149,7 @@
       </c>
     </row>
     <row r="448" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A448" s="44"/>
+      <c r="A448" s="45"/>
       <c r="B448" s="17">
         <v>4</v>
       </c>
@@ -64123,7 +64279,7 @@
       </c>
     </row>
     <row r="449" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A449" s="44"/>
+      <c r="A449" s="45"/>
       <c r="B449" s="17">
         <v>5</v>
       </c>
@@ -64253,7 +64409,7 @@
       </c>
     </row>
     <row r="450" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A450" s="44"/>
+      <c r="A450" s="45"/>
       <c r="B450" s="17">
         <v>6</v>
       </c>
@@ -64383,7 +64539,7 @@
       </c>
     </row>
     <row r="451" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A451" s="44"/>
+      <c r="A451" s="45"/>
       <c r="B451" s="17">
         <v>7</v>
       </c>
@@ -64513,7 +64669,7 @@
       </c>
     </row>
     <row r="452" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A452" s="44"/>
+      <c r="A452" s="45"/>
       <c r="B452" s="17">
         <v>8</v>
       </c>
@@ -64643,7 +64799,7 @@
       </c>
     </row>
     <row r="453" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A453" s="44"/>
+      <c r="A453" s="45"/>
       <c r="B453" s="17">
         <v>9</v>
       </c>
@@ -64773,7 +64929,7 @@
       </c>
     </row>
     <row r="454" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A454" s="44"/>
+      <c r="A454" s="45"/>
       <c r="B454" s="17">
         <v>10</v>
       </c>
@@ -64903,7 +65059,7 @@
       </c>
     </row>
     <row r="455" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A455" s="44"/>
+      <c r="A455" s="45"/>
       <c r="B455" s="17">
         <v>11</v>
       </c>
@@ -65033,7 +65189,7 @@
       </c>
     </row>
     <row r="456" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A456" s="44"/>
+      <c r="A456" s="45"/>
       <c r="B456" s="17">
         <v>12</v>
       </c>
@@ -65163,7 +65319,7 @@
       </c>
     </row>
     <row r="457" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A457" s="44"/>
+      <c r="A457" s="45"/>
       <c r="B457" s="17">
         <v>13</v>
       </c>
@@ -65293,7 +65449,7 @@
       </c>
     </row>
     <row r="458" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A458" s="44"/>
+      <c r="A458" s="45"/>
       <c r="B458" s="17">
         <v>14</v>
       </c>
@@ -65423,7 +65579,7 @@
       </c>
     </row>
     <row r="459" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A459" s="44"/>
+      <c r="A459" s="45"/>
       <c r="B459" s="17">
         <v>15</v>
       </c>
@@ -65553,7 +65709,7 @@
       </c>
     </row>
     <row r="460" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A460" s="44"/>
+      <c r="A460" s="45"/>
       <c r="B460" s="17">
         <v>16</v>
       </c>
@@ -65683,7 +65839,7 @@
       </c>
     </row>
     <row r="461" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A461" s="44"/>
+      <c r="A461" s="45"/>
       <c r="B461" s="17">
         <v>17</v>
       </c>
@@ -65813,7 +65969,7 @@
       </c>
     </row>
     <row r="462" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A462" s="44"/>
+      <c r="A462" s="45"/>
       <c r="B462" s="17">
         <v>18</v>
       </c>
@@ -65943,7 +66099,7 @@
       </c>
     </row>
     <row r="463" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A463" s="44"/>
+      <c r="A463" s="45"/>
       <c r="B463" s="17">
         <v>19</v>
       </c>
@@ -66073,7 +66229,7 @@
       </c>
     </row>
     <row r="464" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A464" s="44"/>
+      <c r="A464" s="45"/>
       <c r="B464" s="17">
         <v>20</v>
       </c>
@@ -66203,7 +66359,7 @@
       </c>
     </row>
     <row r="465" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A465" s="44"/>
+      <c r="A465" s="45"/>
       <c r="B465" s="17">
         <v>21</v>
       </c>
@@ -66333,7 +66489,7 @@
       </c>
     </row>
     <row r="466" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A466" s="44"/>
+      <c r="A466" s="45"/>
       <c r="B466" s="17">
         <v>22</v>
       </c>
@@ -66463,7 +66619,7 @@
       </c>
     </row>
     <row r="467" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A467" s="44"/>
+      <c r="A467" s="45"/>
       <c r="B467" s="17">
         <v>23</v>
       </c>
@@ -66593,7 +66749,7 @@
       </c>
     </row>
     <row r="468" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A468" s="44"/>
+      <c r="A468" s="45"/>
       <c r="B468" s="17">
         <v>24</v>
       </c>
@@ -66723,7 +66879,7 @@
       </c>
     </row>
     <row r="469" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A469" s="44"/>
+      <c r="A469" s="45"/>
       <c r="B469" s="17">
         <v>25</v>
       </c>
@@ -66853,7 +67009,7 @@
       </c>
     </row>
     <row r="470" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A470" s="44"/>
+      <c r="A470" s="45"/>
       <c r="B470" s="17">
         <v>26</v>
       </c>
@@ -66983,7 +67139,7 @@
       </c>
     </row>
     <row r="471" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A471" s="44"/>
+      <c r="A471" s="45"/>
       <c r="B471" s="17">
         <v>27</v>
       </c>
@@ -67113,7 +67269,7 @@
       </c>
     </row>
     <row r="472" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A472" s="44"/>
+      <c r="A472" s="45"/>
       <c r="B472" s="17">
         <v>28</v>
       </c>
@@ -67243,7 +67399,7 @@
       </c>
     </row>
     <row r="473" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A473" s="44"/>
+      <c r="A473" s="45"/>
       <c r="B473" s="17">
         <v>29</v>
       </c>
@@ -67373,7 +67529,7 @@
       </c>
     </row>
     <row r="474" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A474" s="44"/>
+      <c r="A474" s="45"/>
       <c r="B474" s="17">
         <v>30</v>
       </c>
@@ -67503,7 +67659,7 @@
       </c>
     </row>
     <row r="475" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A475" s="44"/>
+      <c r="A475" s="45"/>
       <c r="B475" s="17">
         <v>31</v>
       </c>
@@ -67633,7 +67789,7 @@
       </c>
     </row>
     <row r="476" spans="1:373" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A476" s="44"/>
+      <c r="A476" s="45"/>
       <c r="B476" s="21">
         <v>32</v>
       </c>
@@ -68092,7 +68248,7 @@
       <c r="NI476" s="5"/>
     </row>
     <row r="477" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A477" s="44"/>
+      <c r="A477" s="45"/>
       <c r="B477" s="17">
         <v>33</v>
       </c>
@@ -68221,7 +68377,7 @@
       </c>
     </row>
     <row r="478" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A478" s="44"/>
+      <c r="A478" s="45"/>
       <c r="B478" s="17">
         <v>34</v>
       </c>
@@ -68350,7 +68506,7 @@
       </c>
     </row>
     <row r="479" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A479" s="44"/>
+      <c r="A479" s="45"/>
       <c r="B479" s="17">
         <v>35</v>
       </c>
@@ -68479,7 +68635,7 @@
       </c>
     </row>
     <row r="480" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A480" s="44"/>
+      <c r="A480" s="45"/>
       <c r="B480" s="17">
         <v>36</v>
       </c>
@@ -68608,7 +68764,7 @@
       </c>
     </row>
     <row r="481" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A481" s="44"/>
+      <c r="A481" s="45"/>
       <c r="B481" s="17">
         <v>37</v>
       </c>
@@ -68737,7 +68893,7 @@
       </c>
     </row>
     <row r="482" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A482" s="44"/>
+      <c r="A482" s="45"/>
       <c r="B482" s="17">
         <v>38</v>
       </c>
@@ -68866,7 +69022,7 @@
       </c>
     </row>
     <row r="483" spans="1:43" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A483" s="44"/>
+      <c r="A483" s="45"/>
       <c r="B483" s="17">
         <v>39</v>
       </c>
@@ -68995,7 +69151,7 @@
       </c>
     </row>
     <row r="484" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A484" s="45"/>
+      <c r="A484" s="46"/>
       <c r="B484" s="27">
         <v>40</v>
       </c>
@@ -69229,6 +69385,7 @@
     <row r="588" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A285:A324"/>
     <mergeCell ref="A325:A364"/>
     <mergeCell ref="A365:A404"/>
     <mergeCell ref="A405:A444"/>
@@ -69245,7 +69402,6 @@
     <mergeCell ref="A165:A204"/>
     <mergeCell ref="A205:A244"/>
     <mergeCell ref="A245:A284"/>
-    <mergeCell ref="A285:A324"/>
   </mergeCells>
   <conditionalFormatting sqref="AI2:AQ2">
     <cfRule type="colorScale" priority="37">

</xml_diff>